<commit_message>
replace grouptc-hash-v2 to grouptc-cuckoo
</commit_message>
<xml_diff>
--- a/excel/grouptc_hs_vs_trust_time.xlsx
+++ b/excel/grouptc_hs_vs_trust_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Datasets</t>
   </si>
@@ -25,18 +25,36 @@
     <t>grouptc_hs_small degree vertex hash table construction time</t>
   </si>
   <si>
+    <t>grouptc_hs_large degree vertex total time</t>
+  </si>
+  <si>
+    <t>grouptc_hs_large degree vertex hash table construction time</t>
+  </si>
+  <si>
     <t>grouptc_hs_small degree vertex hash search time</t>
   </si>
   <si>
+    <t>grouptc_hs_large degree vertex hash search time</t>
+  </si>
+  <si>
     <t>trust_small degree vertex total time</t>
   </si>
   <si>
     <t>trust_small degree vertex hash table construction time</t>
   </si>
   <si>
+    <t>trust_large degree vertex total time</t>
+  </si>
+  <si>
+    <t>trust_large degree vertex hash table construction time</t>
+  </si>
+  <si>
     <t>trust_small degree vertex hash search time</t>
   </si>
   <si>
+    <t>trust_large degree vertex hash search time</t>
+  </si>
+  <si>
     <t>baseline</t>
   </si>
   <si>
@@ -49,6 +67,15 @@
     <t>small degree vertex hash search time_speedup</t>
   </si>
   <si>
+    <t>large degree vertex total time_speedup</t>
+  </si>
+  <si>
+    <t>large degree vertex hash table construction time_speedup</t>
+  </si>
+  <si>
+    <t>large degree vertex hash search time_speedup</t>
+  </si>
+  <si>
     <t>vertex_count</t>
   </si>
   <si>
@@ -73,6 +100,9 @@
     <t>small degree vertex avg degree</t>
   </si>
   <si>
+    <t>large degree vertex avg degree</t>
+  </si>
+  <si>
     <t>WN</t>
   </si>
   <si>
@@ -176,6 +206,9 @@
   </si>
   <si>
     <t>s24-e32</t>
+  </si>
+  <si>
+    <t>-inf</t>
   </si>
 </sst>
 </file>
@@ -533,13 +566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S43"/>
+  <dimension ref="A1:AC43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:29">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,10 +630,40 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:29">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>0.241</v>
@@ -609,57 +672,87 @@
         <v>0.092</v>
       </c>
       <c r="D2">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="E2">
+        <v>0.056</v>
+      </c>
+      <c r="F2">
         <v>0.149</v>
       </c>
-      <c r="E2">
+      <c r="G2">
+        <v>0.029</v>
+      </c>
+      <c r="H2">
         <v>0.444</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>0.154</v>
       </c>
-      <c r="G2">
+      <c r="J2">
+        <v>0.463</v>
+      </c>
+      <c r="K2">
+        <v>0.039</v>
+      </c>
+      <c r="L2">
         <v>0.29</v>
       </c>
-      <c r="H2">
+      <c r="M2">
+        <v>0.424</v>
+      </c>
+      <c r="N2">
         <v>1</v>
       </c>
-      <c r="I2">
+      <c r="O2">
         <v>1.842323651452282</v>
       </c>
-      <c r="J2">
+      <c r="P2">
         <v>1.673913043478261</v>
       </c>
-      <c r="K2">
+      <c r="Q2">
         <v>1.946308724832215</v>
       </c>
-      <c r="L2">
+      <c r="R2">
+        <v>5.447058823529411</v>
+      </c>
+      <c r="S2">
+        <v>0.6964285714285714</v>
+      </c>
+      <c r="T2">
+        <v>14.62068965517241</v>
+      </c>
+      <c r="U2">
         <v>325729</v>
       </c>
-      <c r="M2">
+      <c r="V2">
         <v>1090108</v>
       </c>
-      <c r="N2">
+      <c r="W2">
         <v>6.693343239318574</v>
       </c>
-      <c r="O2">
+      <c r="X2">
         <v>487</v>
       </c>
-      <c r="P2">
+      <c r="Y2">
         <v>62122</v>
       </c>
-      <c r="Q2">
+      <c r="Z2">
         <v>151666</v>
       </c>
-      <c r="R2">
+      <c r="AA2">
         <v>918795</v>
       </c>
-      <c r="S2">
+      <c r="AB2">
         <v>11.33322749852823</v>
       </c>
+      <c r="AC2">
+        <v>255.1211498973306</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:29">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>0.199</v>
@@ -668,57 +761,87 @@
         <v>0.08399999999999999</v>
       </c>
       <c r="D3">
+        <v>0.054</v>
+      </c>
+      <c r="E3">
+        <v>0.04500000000000001</v>
+      </c>
+      <c r="F3">
         <v>0.115</v>
       </c>
-      <c r="E3">
+      <c r="G3">
+        <v>0.008999999999999994</v>
+      </c>
+      <c r="H3">
         <v>0.5419999999999999</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>0.212</v>
       </c>
-      <c r="G3">
+      <c r="J3">
+        <v>0.074</v>
+      </c>
+      <c r="K3">
+        <v>0.037</v>
+      </c>
+      <c r="L3">
         <v>0.33</v>
       </c>
-      <c r="H3">
+      <c r="M3">
+        <v>0.037</v>
+      </c>
+      <c r="N3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="O3">
         <v>2.723618090452261</v>
       </c>
-      <c r="J3">
+      <c r="P3">
         <v>2.523809523809524</v>
       </c>
-      <c r="K3">
+      <c r="Q3">
         <v>2.869565217391303</v>
       </c>
-      <c r="L3">
+      <c r="R3">
+        <v>1.37037037037037</v>
+      </c>
+      <c r="S3">
+        <v>0.8222222222222221</v>
+      </c>
+      <c r="T3">
+        <v>4.111111111111113</v>
+      </c>
+      <c r="U3">
         <v>317080</v>
       </c>
-      <c r="M3">
+      <c r="V3">
         <v>1049866</v>
       </c>
-      <c r="N3">
+      <c r="W3">
         <v>6.622089062697111</v>
       </c>
-      <c r="O3">
+      <c r="X3">
         <v>14</v>
       </c>
-      <c r="P3">
+      <c r="Y3">
         <v>1492</v>
       </c>
-      <c r="Q3">
+      <c r="Z3">
         <v>242509</v>
       </c>
-      <c r="R3">
+      <c r="AA3">
         <v>977594</v>
       </c>
-      <c r="S3">
+      <c r="AB3">
         <v>8.050491762716756</v>
       </c>
+      <c r="AC3">
+        <v>213.1428571428571</v>
+      </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:29">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <v>0.381</v>
@@ -727,57 +850,81 @@
         <v>0.126</v>
       </c>
       <c r="D4">
+        <v>0.046</v>
+      </c>
+      <c r="E4">
+        <v>0.046</v>
+      </c>
+      <c r="F4">
         <v>0.255</v>
       </c>
-      <c r="E4">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>0.903</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>0.32</v>
       </c>
-      <c r="G4">
+      <c r="J4">
+        <v>0.034</v>
+      </c>
+      <c r="K4">
+        <v>0.034</v>
+      </c>
+      <c r="L4">
         <v>0.583</v>
       </c>
-      <c r="H4">
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
         <v>1</v>
       </c>
-      <c r="I4">
+      <c r="O4">
         <v>2.370078740157481</v>
       </c>
-      <c r="J4">
+      <c r="P4">
         <v>2.53968253968254</v>
       </c>
-      <c r="K4">
+      <c r="Q4">
         <v>2.286274509803921</v>
       </c>
-      <c r="L4">
+      <c r="R4">
+        <v>0.7391304347826088</v>
+      </c>
+      <c r="S4">
+        <v>0.7391304347826088</v>
+      </c>
+      <c r="U4">
         <v>403394</v>
       </c>
-      <c r="M4">
+      <c r="V4">
         <v>2443408</v>
       </c>
-      <c r="N4">
+      <c r="W4">
         <v>12.11425058379649</v>
       </c>
-      <c r="O4">
+      <c r="X4">
         <v>0</v>
       </c>
-      <c r="P4">
+      <c r="Y4">
         <v>0</v>
       </c>
-      <c r="Q4">
+      <c r="Z4">
         <v>377343</v>
       </c>
-      <c r="R4">
+      <c r="AA4">
         <v>2421872</v>
       </c>
-      <c r="S4">
+      <c r="AB4">
         <v>12.83644853621241</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:29">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>0.358</v>
@@ -786,57 +933,84 @@
         <v>0.115</v>
       </c>
       <c r="D5">
+        <v>0.044</v>
+      </c>
+      <c r="E5">
+        <v>0.04500000000000001</v>
+      </c>
+      <c r="F5">
         <v>0.243</v>
       </c>
-      <c r="E5">
+      <c r="G5">
+        <v>-0.001000000000000008</v>
+      </c>
+      <c r="H5">
         <v>0.945</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>0.6489999999999999</v>
       </c>
-      <c r="G5">
+      <c r="J5">
+        <v>0.032</v>
+      </c>
+      <c r="K5">
+        <v>0.033</v>
+      </c>
+      <c r="L5">
         <v>0.296</v>
       </c>
-      <c r="H5">
+      <c r="M5">
+        <v>-0.001000000000000001</v>
+      </c>
+      <c r="N5">
         <v>1</v>
       </c>
-      <c r="I5">
+      <c r="O5">
         <v>2.639664804469274</v>
       </c>
-      <c r="J5">
+      <c r="P5">
         <v>5.643478260869564</v>
       </c>
-      <c r="K5">
+      <c r="Q5">
         <v>1.218106995884774</v>
       </c>
-      <c r="L5">
+      <c r="R5">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="S5">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="T5">
+        <v>0.9999999999999931</v>
+      </c>
+      <c r="U5">
         <v>1965206</v>
       </c>
-      <c r="M5">
+      <c r="V5">
         <v>2766607</v>
       </c>
-      <c r="N5">
+      <c r="W5">
         <v>2.815589816029465</v>
       </c>
-      <c r="O5">
+      <c r="X5">
         <v>0</v>
       </c>
-      <c r="P5">
+      <c r="Y5">
         <v>0</v>
       </c>
-      <c r="Q5">
+      <c r="Z5">
         <v>856203</v>
       </c>
-      <c r="R5">
+      <c r="AA5">
         <v>1928091</v>
       </c>
-      <c r="S5">
+      <c r="AB5">
         <v>4.503817435818375</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:29">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>1.032</v>
@@ -845,57 +1019,87 @@
         <v>0.161</v>
       </c>
       <c r="D6">
+        <v>0.203</v>
+      </c>
+      <c r="E6">
+        <v>0.094</v>
+      </c>
+      <c r="F6">
         <v>0.871</v>
       </c>
-      <c r="E6">
+      <c r="G6">
+        <v>0.109</v>
+      </c>
+      <c r="H6">
         <v>3.856</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>0.481</v>
       </c>
-      <c r="G6">
+      <c r="J6">
+        <v>0.747</v>
+      </c>
+      <c r="K6">
+        <v>0.039</v>
+      </c>
+      <c r="L6">
         <v>3.375</v>
       </c>
-      <c r="H6">
+      <c r="M6">
+        <v>0.708</v>
+      </c>
+      <c r="N6">
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="O6">
         <v>3.736434108527132</v>
       </c>
-      <c r="J6">
+      <c r="P6">
         <v>2.987577639751553</v>
       </c>
-      <c r="K6">
+      <c r="Q6">
         <v>3.874856486796785</v>
       </c>
-      <c r="L6">
+      <c r="R6">
+        <v>3.679802955665024</v>
+      </c>
+      <c r="S6">
+        <v>0.4148936170212766</v>
+      </c>
+      <c r="T6">
+        <v>6.495412844036696</v>
+      </c>
+      <c r="U6">
         <v>2394385</v>
       </c>
-      <c r="M6">
+      <c r="V6">
         <v>4659565</v>
       </c>
-      <c r="N6">
+      <c r="W6">
         <v>3.892076671044966</v>
       </c>
-      <c r="O6">
+      <c r="X6">
         <v>1411</v>
       </c>
-      <c r="P6">
+      <c r="Y6">
         <v>203200</v>
       </c>
-      <c r="Q6">
+      <c r="Z6">
         <v>621012</v>
       </c>
-      <c r="R6">
+      <c r="AA6">
         <v>2888957</v>
       </c>
-      <c r="S6">
+      <c r="AB6">
         <v>8.669311379419982</v>
       </c>
+      <c r="AC6">
+        <v>288.0226789510985</v>
+      </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:29">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>1.099</v>
@@ -904,57 +1108,87 @@
         <v>0.221</v>
       </c>
       <c r="D7">
+        <v>0.075</v>
+      </c>
+      <c r="E7">
+        <v>0.067</v>
+      </c>
+      <c r="F7">
         <v>0.878</v>
       </c>
-      <c r="E7">
+      <c r="G7">
+        <v>0.007999999999999993</v>
+      </c>
+      <c r="H7">
         <v>2.103</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>0.648</v>
       </c>
-      <c r="G7">
+      <c r="J7">
+        <v>0.066</v>
+      </c>
+      <c r="K7">
+        <v>0.032</v>
+      </c>
+      <c r="L7">
         <v>1.455</v>
       </c>
-      <c r="H7">
+      <c r="M7">
+        <v>0.034</v>
+      </c>
+      <c r="N7">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="O7">
         <v>1.913557779799818</v>
       </c>
-      <c r="J7">
+      <c r="P7">
         <v>2.932126696832579</v>
       </c>
-      <c r="K7">
+      <c r="Q7">
         <v>1.657175398633257</v>
       </c>
-      <c r="L7">
+      <c r="R7">
+        <v>0.8800000000000001</v>
+      </c>
+      <c r="S7">
+        <v>0.4776119402985075</v>
+      </c>
+      <c r="T7">
+        <v>4.250000000000004</v>
+      </c>
+      <c r="U7">
         <v>1224346</v>
       </c>
-      <c r="M7">
+      <c r="V7">
         <v>5369472</v>
       </c>
-      <c r="N7">
+      <c r="W7">
         <v>8.771167627451717</v>
       </c>
-      <c r="O7">
+      <c r="X7">
         <v>4</v>
       </c>
-      <c r="P7">
+      <c r="Y7">
         <v>406</v>
       </c>
-      <c r="Q7">
+      <c r="Z7">
         <v>848577</v>
       </c>
-      <c r="R7">
+      <c r="AA7">
         <v>5094250</v>
       </c>
-      <c r="S7">
+      <c r="AB7">
         <v>12.00567069656942</v>
       </c>
+      <c r="AC7">
+        <v>203</v>
+      </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:29">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <v>1.138</v>
@@ -963,57 +1197,87 @@
         <v>0.279</v>
       </c>
       <c r="D8">
+        <v>0.177</v>
+      </c>
+      <c r="E8">
+        <v>0.111</v>
+      </c>
+      <c r="F8">
         <v>0.8589999999999999</v>
       </c>
-      <c r="E8">
+      <c r="G8">
+        <v>0.06599999999999999</v>
+      </c>
+      <c r="H8">
         <v>1.828</v>
       </c>
-      <c r="F8">
+      <c r="I8">
         <v>0.476</v>
       </c>
-      <c r="G8">
+      <c r="J8">
+        <v>0.7240000000000001</v>
+      </c>
+      <c r="K8">
+        <v>0.042</v>
+      </c>
+      <c r="L8">
         <v>1.352</v>
       </c>
-      <c r="H8">
+      <c r="M8">
+        <v>0.6820000000000001</v>
+      </c>
+      <c r="N8">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="O8">
         <v>1.606326889279438</v>
       </c>
-      <c r="J8">
+      <c r="P8">
         <v>1.706093189964158</v>
       </c>
-      <c r="K8">
+      <c r="Q8">
         <v>1.573923166472643</v>
       </c>
-      <c r="L8">
+      <c r="R8">
+        <v>4.09039548022599</v>
+      </c>
+      <c r="S8">
+        <v>0.3783783783783783</v>
+      </c>
+      <c r="T8">
+        <v>10.33333333333334</v>
+      </c>
+      <c r="U8">
         <v>685230</v>
       </c>
-      <c r="M8">
+      <c r="V8">
         <v>6649470</v>
       </c>
-      <c r="N8">
+      <c r="W8">
         <v>19.40799439604221</v>
       </c>
-      <c r="O8">
+      <c r="X8">
         <v>1854</v>
       </c>
-      <c r="P8">
+      <c r="Y8">
         <v>209701</v>
       </c>
-      <c r="Q8">
+      <c r="Z8">
         <v>608489</v>
       </c>
-      <c r="R8">
+      <c r="AA8">
         <v>6581031</v>
       </c>
-      <c r="S8">
+      <c r="AB8">
         <v>21.00548105532981</v>
       </c>
+      <c r="AC8">
+        <v>226.2146709816613</v>
+      </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:29">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B9">
         <v>2.165</v>
@@ -1022,57 +1286,87 @@
         <v>0.385</v>
       </c>
       <c r="D9">
+        <v>0.156</v>
+      </c>
+      <c r="E9">
+        <v>0.112</v>
+      </c>
+      <c r="F9">
         <v>1.78</v>
       </c>
-      <c r="E9">
+      <c r="G9">
+        <v>0.044</v>
+      </c>
+      <c r="H9">
         <v>4.464</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>1.072</v>
       </c>
-      <c r="G9">
+      <c r="J9">
+        <v>0.5720000000000001</v>
+      </c>
+      <c r="K9">
+        <v>0.036</v>
+      </c>
+      <c r="L9">
         <v>3.392</v>
       </c>
-      <c r="H9">
+      <c r="M9">
+        <v>0.536</v>
+      </c>
+      <c r="N9">
         <v>1</v>
       </c>
-      <c r="I9">
+      <c r="O9">
         <v>2.06189376443418</v>
       </c>
-      <c r="J9">
+      <c r="P9">
         <v>2.784415584415585</v>
       </c>
-      <c r="K9">
+      <c r="Q9">
         <v>1.90561797752809</v>
       </c>
-      <c r="L9">
+      <c r="R9">
+        <v>3.666666666666667</v>
+      </c>
+      <c r="S9">
+        <v>0.3214285714285715</v>
+      </c>
+      <c r="T9">
+        <v>12.18181818181818</v>
+      </c>
+      <c r="U9">
         <v>1696415</v>
       </c>
-      <c r="M9">
+      <c r="V9">
         <v>11095298</v>
       </c>
-      <c r="N9">
+      <c r="W9">
         <v>13.08087702596358</v>
       </c>
-      <c r="O9">
+      <c r="X9">
         <v>988</v>
       </c>
-      <c r="P9">
+      <c r="Y9">
         <v>116340</v>
       </c>
-      <c r="Q9">
+      <c r="Z9">
         <v>1423165</v>
       </c>
-      <c r="R9">
+      <c r="AA9">
         <v>10832625</v>
       </c>
-      <c r="S9">
+      <c r="AB9">
         <v>15.07025496826344</v>
       </c>
+      <c r="AC9">
+        <v>235.5060728744939</v>
+      </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:29">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B10">
         <v>4.61</v>
@@ -1081,57 +1375,84 @@
         <v>0.484</v>
       </c>
       <c r="D10">
+        <v>0.103</v>
+      </c>
+      <c r="E10">
+        <v>0.102</v>
+      </c>
+      <c r="F10">
         <v>4.126</v>
       </c>
-      <c r="E10">
+      <c r="G10">
+        <v>0.001000000000000001</v>
+      </c>
+      <c r="H10">
         <v>7.976999999999999</v>
       </c>
-      <c r="F10">
+      <c r="I10">
         <v>2.182</v>
       </c>
-      <c r="G10">
+      <c r="J10">
+        <v>0.032</v>
+      </c>
+      <c r="K10">
+        <v>0.032</v>
+      </c>
+      <c r="L10">
         <v>5.795</v>
       </c>
-      <c r="H10">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
         <v>1</v>
       </c>
-      <c r="I10">
+      <c r="O10">
         <v>1.730368763557484</v>
       </c>
-      <c r="J10">
+      <c r="P10">
         <v>4.508264462809917</v>
       </c>
-      <c r="K10">
+      <c r="Q10">
         <v>1.404507998061076</v>
       </c>
-      <c r="L10">
+      <c r="R10">
+        <v>0.3106796116504855</v>
+      </c>
+      <c r="S10">
+        <v>0.3137254901960785</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
         <v>3774768</v>
       </c>
-      <c r="M10">
+      <c r="V10">
         <v>16518947</v>
       </c>
-      <c r="N10">
+      <c r="W10">
         <v>8.752297889565664</v>
       </c>
-      <c r="O10">
+      <c r="X10">
         <v>0</v>
       </c>
-      <c r="P10">
+      <c r="Y10">
         <v>0</v>
       </c>
-      <c r="Q10">
+      <c r="Z10">
         <v>2944946</v>
       </c>
-      <c r="R10">
+      <c r="AA10">
         <v>15745211</v>
       </c>
-      <c r="S10">
+      <c r="AB10">
         <v>10.69303885368356</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:29">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B11">
         <v>7.163</v>
@@ -1140,57 +1461,84 @@
         <v>0.642</v>
       </c>
       <c r="D11">
+        <v>0.103</v>
+      </c>
+      <c r="E11">
+        <v>0.104</v>
+      </c>
+      <c r="F11">
         <v>6.521</v>
       </c>
-      <c r="E11">
+      <c r="G11">
+        <v>-0.001000000000000001</v>
+      </c>
+      <c r="H11">
         <v>12.62</v>
       </c>
-      <c r="F11">
+      <c r="I11">
         <v>1.117</v>
       </c>
-      <c r="G11">
+      <c r="J11">
+        <v>0.032</v>
+      </c>
+      <c r="K11">
+        <v>0.032</v>
+      </c>
+      <c r="L11">
         <v>11.503</v>
       </c>
-      <c r="H11">
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
         <v>1</v>
       </c>
-      <c r="I11">
+      <c r="O11">
         <v>1.761831634789892</v>
       </c>
-      <c r="J11">
+      <c r="P11">
         <v>1.7398753894081</v>
       </c>
-      <c r="K11">
+      <c r="Q11">
         <v>1.763993252568624</v>
       </c>
-      <c r="L11">
+      <c r="R11">
+        <v>0.3106796116504855</v>
+      </c>
+      <c r="S11">
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="T11">
+        <v>-0</v>
+      </c>
+      <c r="U11">
         <v>1632803</v>
       </c>
-      <c r="M11">
+      <c r="V11">
         <v>22301964</v>
       </c>
-      <c r="N11">
+      <c r="W11">
         <v>27.31739713854029</v>
       </c>
-      <c r="O11">
+      <c r="X11">
         <v>0</v>
       </c>
-      <c r="P11">
+      <c r="Y11">
         <v>0</v>
       </c>
-      <c r="Q11">
+      <c r="Z11">
         <v>1462551</v>
       </c>
-      <c r="R11">
+      <c r="AA11">
         <v>22132301</v>
       </c>
-      <c r="S11">
+      <c r="AB11">
         <v>30.2653391232169</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:29">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B12">
         <v>16.147</v>
@@ -1199,57 +1547,87 @@
         <v>0.628</v>
       </c>
       <c r="D12">
+        <v>5.15</v>
+      </c>
+      <c r="E12">
+        <v>0.43</v>
+      </c>
+      <c r="F12">
         <v>15.519</v>
       </c>
-      <c r="E12">
+      <c r="G12">
+        <v>4.720000000000001</v>
+      </c>
+      <c r="H12">
         <v>33.665</v>
       </c>
-      <c r="F12">
+      <c r="I12">
         <v>1.444</v>
       </c>
-      <c r="G12">
+      <c r="J12">
+        <v>6.728</v>
+      </c>
+      <c r="K12">
+        <v>0.342</v>
+      </c>
+      <c r="L12">
         <v>32.221</v>
       </c>
-      <c r="H12">
+      <c r="M12">
+        <v>6.386</v>
+      </c>
+      <c r="N12">
         <v>1</v>
       </c>
-      <c r="I12">
+      <c r="O12">
         <v>2.08490741314176</v>
       </c>
-      <c r="J12">
+      <c r="P12">
         <v>2.29936305732484</v>
       </c>
-      <c r="K12">
+      <c r="Q12">
         <v>2.076229138475417</v>
       </c>
-      <c r="L12">
+      <c r="R12">
+        <v>1.306407766990291</v>
+      </c>
+      <c r="S12">
+        <v>0.7953488372093024</v>
+      </c>
+      <c r="T12">
+        <v>1.352966101694915</v>
+      </c>
+      <c r="U12">
         <v>2601977</v>
       </c>
-      <c r="M12">
+      <c r="V12">
         <v>28183518</v>
       </c>
-      <c r="N12">
+      <c r="W12">
         <v>21.66315689954216</v>
       </c>
-      <c r="O12">
+      <c r="X12">
         <v>37378</v>
       </c>
-      <c r="P12">
+      <c r="Y12">
         <v>5559907</v>
       </c>
-      <c r="Q12">
+      <c r="Z12">
         <v>1947518</v>
       </c>
-      <c r="R12">
+      <c r="AA12">
         <v>27552833</v>
       </c>
-      <c r="S12">
+      <c r="AB12">
         <v>23.02755400127739</v>
       </c>
+      <c r="AC12">
+        <v>297.4962277275403</v>
+      </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:29">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B13">
         <v>9.061</v>
@@ -1258,57 +1636,87 @@
         <v>0.889</v>
       </c>
       <c r="D13">
+        <v>0.777</v>
+      </c>
+      <c r="E13">
+        <v>0.178</v>
+      </c>
+      <c r="F13">
         <v>8.172000000000001</v>
       </c>
-      <c r="E13">
+      <c r="G13">
+        <v>0.599</v>
+      </c>
+      <c r="H13">
         <v>17.683</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <v>2.335</v>
       </c>
-      <c r="G13">
+      <c r="J13">
+        <v>1.405</v>
+      </c>
+      <c r="K13">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="L13">
         <v>15.348</v>
       </c>
-      <c r="H13">
+      <c r="M13">
+        <v>1.32</v>
+      </c>
+      <c r="N13">
         <v>1</v>
       </c>
-      <c r="I13">
+      <c r="O13">
         <v>1.951550601478865</v>
       </c>
-      <c r="J13">
+      <c r="P13">
         <v>2.626546681664792</v>
       </c>
-      <c r="K13">
+      <c r="Q13">
         <v>1.878120411160058</v>
       </c>
-      <c r="L13">
+      <c r="R13">
+        <v>1.808236808236808</v>
+      </c>
+      <c r="S13">
+        <v>0.4775280898876405</v>
+      </c>
+      <c r="T13">
+        <v>2.203672787979967</v>
+      </c>
+      <c r="U13">
         <v>3997962</v>
       </c>
-      <c r="M13">
+      <c r="V13">
         <v>34681189</v>
       </c>
-      <c r="N13">
+      <c r="W13">
         <v>17.34943403664167</v>
       </c>
-      <c r="O13">
+      <c r="X13">
         <v>9274</v>
       </c>
-      <c r="P13">
+      <c r="Y13">
         <v>1380556</v>
       </c>
-      <c r="Q13">
+      <c r="Z13">
         <v>3132157</v>
       </c>
-      <c r="R13">
+      <c r="AA13">
         <v>33823008</v>
       </c>
-      <c r="S13">
+      <c r="AB13">
         <v>20.77724461659307</v>
       </c>
+      <c r="AC13">
+        <v>297.7261160232909</v>
+      </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:29">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B14">
         <v>12.375</v>
@@ -1317,57 +1725,87 @@
         <v>1.037</v>
       </c>
       <c r="D14">
+        <v>1.619</v>
+      </c>
+      <c r="E14">
+        <v>0.265</v>
+      </c>
+      <c r="F14">
         <v>11.338</v>
       </c>
-      <c r="E14">
+      <c r="G14">
+        <v>1.354</v>
+      </c>
+      <c r="H14">
         <v>23.156</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <v>2.734</v>
       </c>
-      <c r="G14">
+      <c r="J14">
+        <v>2.535</v>
+      </c>
+      <c r="K14">
+        <v>0.185</v>
+      </c>
+      <c r="L14">
         <v>20.422</v>
       </c>
-      <c r="H14">
+      <c r="M14">
+        <v>2.35</v>
+      </c>
+      <c r="N14">
         <v>1</v>
       </c>
-      <c r="I14">
+      <c r="O14">
         <v>1.871191919191919</v>
       </c>
-      <c r="J14">
+      <c r="P14">
         <v>2.636451301832209</v>
       </c>
-      <c r="K14">
+      <c r="Q14">
         <v>1.801199506085729</v>
       </c>
-      <c r="L14">
+      <c r="R14">
+        <v>1.565781346510192</v>
+      </c>
+      <c r="S14">
+        <v>0.6981132075471698</v>
+      </c>
+      <c r="T14">
+        <v>1.735598227474151</v>
+      </c>
+      <c r="U14">
         <v>4847571</v>
       </c>
-      <c r="M14">
+      <c r="V14">
         <v>42851237</v>
       </c>
-      <c r="N14">
+      <c r="W14">
         <v>17.67946751063574</v>
       </c>
-      <c r="O14">
+      <c r="X14">
         <v>18936</v>
       </c>
-      <c r="P14">
+      <c r="Y14">
         <v>2875108</v>
       </c>
-      <c r="Q14">
+      <c r="Z14">
         <v>3680794</v>
       </c>
-      <c r="R14">
+      <c r="AA14">
         <v>41695681</v>
       </c>
-      <c r="S14">
+      <c r="AB14">
         <v>21.202664330512</v>
       </c>
+      <c r="AC14">
+        <v>303.6658217152514</v>
+      </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:29">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>4.564</v>
@@ -1376,57 +1814,84 @@
         <v>0.983</v>
       </c>
       <c r="D15">
+        <v>0.103</v>
+      </c>
+      <c r="E15">
+        <v>0.103</v>
+      </c>
+      <c r="F15">
         <v>3.581</v>
       </c>
-      <c r="E15">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>22.629</v>
       </c>
-      <c r="F15">
+      <c r="I15">
         <v>14.079</v>
       </c>
-      <c r="G15">
+      <c r="J15">
+        <v>0.032</v>
+      </c>
+      <c r="K15">
+        <v>0.033</v>
+      </c>
+      <c r="L15">
         <v>8.550000000000002</v>
       </c>
-      <c r="H15">
+      <c r="M15">
+        <v>-0.001000000000000001</v>
+      </c>
+      <c r="N15">
         <v>1</v>
       </c>
-      <c r="I15">
+      <c r="O15">
         <v>4.958150744960562</v>
       </c>
-      <c r="J15">
+      <c r="P15">
         <v>14.32248219735503</v>
       </c>
-      <c r="K15">
+      <c r="Q15">
         <v>2.387601228707066</v>
       </c>
-      <c r="L15">
+      <c r="R15">
+        <v>0.3106796116504855</v>
+      </c>
+      <c r="S15">
+        <v>0.3203883495145631</v>
+      </c>
+      <c r="T15" t="s">
+        <v>64</v>
+      </c>
+      <c r="U15">
         <v>55042369</v>
       </c>
-      <c r="M15">
+      <c r="V15">
         <v>58608800</v>
       </c>
-      <c r="N15">
+      <c r="W15">
         <v>2.129588572032574</v>
       </c>
-      <c r="O15">
+      <c r="X15">
         <v>0</v>
       </c>
-      <c r="P15">
+      <c r="Y15">
         <v>0</v>
       </c>
-      <c r="Q15">
+      <c r="Z15">
         <v>19284842</v>
       </c>
-      <c r="R15">
+      <c r="AA15">
         <v>38751887</v>
       </c>
-      <c r="S15">
+      <c r="AB15">
         <v>4.018895980584129</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:29">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B16">
         <v>52.722</v>
@@ -1435,57 +1900,87 @@
         <v>1.367</v>
       </c>
       <c r="D16">
+        <v>118.771</v>
+      </c>
+      <c r="E16">
+        <v>2.639</v>
+      </c>
+      <c r="F16">
         <v>51.355</v>
       </c>
-      <c r="E16">
+      <c r="G16">
+        <v>116.132</v>
+      </c>
+      <c r="H16">
         <v>103.449</v>
       </c>
-      <c r="F16">
+      <c r="I16">
         <v>1.297</v>
       </c>
-      <c r="G16">
+      <c r="J16">
+        <v>170.256</v>
+      </c>
+      <c r="K16">
+        <v>2.396</v>
+      </c>
+      <c r="L16">
         <v>102.152</v>
       </c>
-      <c r="H16">
+      <c r="M16">
+        <v>167.86</v>
+      </c>
+      <c r="N16">
         <v>1</v>
       </c>
-      <c r="I16">
+      <c r="O16">
         <v>1.962160009104359</v>
       </c>
-      <c r="J16">
+      <c r="P16">
         <v>0.9487929773226041</v>
       </c>
-      <c r="K16">
+      <c r="Q16">
         <v>1.989134456236004</v>
       </c>
-      <c r="L16">
+      <c r="R16">
+        <v>1.433481237002298</v>
+      </c>
+      <c r="S16">
+        <v>0.9079196665403563</v>
+      </c>
+      <c r="T16">
+        <v>1.44542417249337</v>
+      </c>
+      <c r="U16">
         <v>1985306</v>
       </c>
-      <c r="M16">
+      <c r="V16">
         <v>114492816</v>
       </c>
-      <c r="N16">
+      <c r="W16">
         <v>115.3402206007537</v>
       </c>
-      <c r="O16">
+      <c r="X16">
         <v>280915</v>
       </c>
-      <c r="P16">
+      <c r="Y16">
         <v>67360442</v>
       </c>
-      <c r="Q16">
+      <c r="Z16">
         <v>1927066</v>
       </c>
-      <c r="R16">
+      <c r="AA16">
         <v>114450945</v>
       </c>
-      <c r="S16">
+      <c r="AB16">
         <v>57.21285957363571</v>
       </c>
+      <c r="AC16">
+        <v>479.578819215777</v>
+      </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:29">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>54.299</v>
@@ -1494,57 +1989,87 @@
         <v>2.333</v>
       </c>
       <c r="D17">
+        <v>21.967</v>
+      </c>
+      <c r="E17">
+        <v>1.181</v>
+      </c>
+      <c r="F17">
         <v>51.966</v>
       </c>
-      <c r="E17">
+      <c r="G17">
+        <v>20.786</v>
+      </c>
+      <c r="H17">
         <v>95.11799999999999</v>
       </c>
-      <c r="F17">
+      <c r="I17">
         <v>2.274</v>
       </c>
-      <c r="G17">
+      <c r="J17">
+        <v>26.272</v>
+      </c>
+      <c r="K17">
+        <v>1.038</v>
+      </c>
+      <c r="L17">
         <v>92.84399999999999</v>
       </c>
-      <c r="H17">
+      <c r="M17">
+        <v>25.234</v>
+      </c>
+      <c r="N17">
         <v>1</v>
       </c>
-      <c r="I17">
+      <c r="O17">
         <v>1.751744967678963</v>
       </c>
-      <c r="J17">
+      <c r="P17">
         <v>0.974710672953279</v>
       </c>
-      <c r="K17">
+      <c r="Q17">
         <v>1.786629719431936</v>
       </c>
-      <c r="L17">
+      <c r="R17">
+        <v>1.1959757818546</v>
+      </c>
+      <c r="S17">
+        <v>0.8789161727349704</v>
+      </c>
+      <c r="T17">
+        <v>1.213990185701915</v>
+      </c>
+      <c r="U17">
         <v>3072441</v>
       </c>
-      <c r="M17">
+      <c r="V17">
         <v>117185083</v>
       </c>
-      <c r="N17">
+      <c r="W17">
         <v>76.28142118921079</v>
       </c>
-      <c r="O17">
+      <c r="X17">
         <v>121341</v>
       </c>
-      <c r="P17">
+      <c r="Y17">
         <v>19727089</v>
       </c>
-      <c r="Q17">
+      <c r="Z17">
         <v>3003794</v>
       </c>
-      <c r="R17">
+      <c r="AA17">
         <v>117116597</v>
       </c>
-      <c r="S17">
+      <c r="AB17">
         <v>67.57404752132992</v>
       </c>
+      <c r="AC17">
+        <v>325.151251431915</v>
+      </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:29">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B18">
         <v>68.15400000000001</v>
@@ -1553,57 +2078,87 @@
         <v>3.458</v>
       </c>
       <c r="D18">
+        <v>10.155</v>
+      </c>
+      <c r="E18">
+        <v>1.125</v>
+      </c>
+      <c r="F18">
         <v>64.69600000000001</v>
       </c>
-      <c r="E18">
+      <c r="G18">
+        <v>9.030000000000001</v>
+      </c>
+      <c r="H18">
         <v>120.842</v>
       </c>
-      <c r="F18">
+      <c r="I18">
         <v>5.06</v>
       </c>
-      <c r="G18">
+      <c r="J18">
+        <v>12.796</v>
+      </c>
+      <c r="K18">
+        <v>1.016</v>
+      </c>
+      <c r="L18">
         <v>115.782</v>
       </c>
-      <c r="H18">
+      <c r="M18">
+        <v>11.78</v>
+      </c>
+      <c r="N18">
         <v>1</v>
       </c>
-      <c r="I18">
+      <c r="O18">
         <v>1.773072747014115</v>
       </c>
-      <c r="J18">
+      <c r="P18">
         <v>1.463273568536726</v>
       </c>
-      <c r="K18">
+      <c r="Q18">
         <v>1.789631507357487</v>
       </c>
-      <c r="L18">
+      <c r="R18">
+        <v>1.260068931560807</v>
+      </c>
+      <c r="S18">
+        <v>0.9031111111111111</v>
+      </c>
+      <c r="T18">
+        <v>1.30454042081949</v>
+      </c>
+      <c r="U18">
         <v>6783976</v>
       </c>
-      <c r="M18">
+      <c r="V18">
         <v>157010940</v>
       </c>
-      <c r="N18">
+      <c r="W18">
         <v>46.28876635176776</v>
       </c>
-      <c r="O18">
+      <c r="X18">
         <v>119735</v>
       </c>
-      <c r="P18">
+      <c r="Y18">
         <v>15839891</v>
       </c>
-      <c r="Q18">
+      <c r="Z18">
         <v>6760186</v>
       </c>
-      <c r="R18">
+      <c r="AA18">
         <v>156987698</v>
       </c>
-      <c r="S18">
+      <c r="AB18">
         <v>42.51151224517732</v>
       </c>
+      <c r="AC18">
+        <v>264.5824696204118</v>
+      </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:29">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B19">
         <v>17.424</v>
@@ -1612,57 +2167,81 @@
         <v>3.573</v>
       </c>
       <c r="D19">
+        <v>0.103</v>
+      </c>
+      <c r="E19">
+        <v>0.103</v>
+      </c>
+      <c r="F19">
         <v>13.851</v>
       </c>
-      <c r="E19">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>90.05199999999999</v>
       </c>
-      <c r="F19">
+      <c r="I19">
         <v>56.877</v>
       </c>
-      <c r="G19">
+      <c r="J19">
+        <v>0.032</v>
+      </c>
+      <c r="K19">
+        <v>0.032</v>
+      </c>
+      <c r="L19">
         <v>33.175</v>
       </c>
-      <c r="H19">
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
         <v>1</v>
       </c>
-      <c r="I19">
+      <c r="O19">
         <v>5.168273645546373</v>
       </c>
-      <c r="J19">
+      <c r="P19">
         <v>15.91855583543241</v>
       </c>
-      <c r="K19">
+      <c r="Q19">
         <v>2.39513392534835</v>
       </c>
-      <c r="L19">
+      <c r="R19">
+        <v>0.3106796116504855</v>
+      </c>
+      <c r="S19">
+        <v>0.3106796116504855</v>
+      </c>
+      <c r="U19">
         <v>214005017</v>
       </c>
-      <c r="M19">
+      <c r="V19">
         <v>232705452</v>
       </c>
-      <c r="N19">
+      <c r="W19">
         <v>2.174766323352129</v>
       </c>
-      <c r="O19">
+      <c r="X19">
         <v>0</v>
       </c>
-      <c r="P19">
+      <c r="Y19">
         <v>0</v>
       </c>
-      <c r="Q19">
+      <c r="Z19">
         <v>78003927</v>
       </c>
-      <c r="R19">
+      <c r="AA19">
         <v>156863950</v>
       </c>
-      <c r="S19">
+      <c r="AB19">
         <v>4.021950074385358</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:29">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B20">
         <v>658.432</v>
@@ -1671,57 +2250,87 @@
         <v>15.506</v>
       </c>
       <c r="D20">
+        <v>2152.196</v>
+      </c>
+      <c r="E20">
+        <v>18.526</v>
+      </c>
+      <c r="F20">
         <v>642.926</v>
       </c>
-      <c r="E20">
+      <c r="G20">
+        <v>2133.67</v>
+      </c>
+      <c r="H20">
         <v>1052.011</v>
       </c>
-      <c r="F20">
+      <c r="I20">
         <v>28.425</v>
       </c>
-      <c r="G20">
+      <c r="J20">
+        <v>2553.767</v>
+      </c>
+      <c r="K20">
+        <v>16.152</v>
+      </c>
+      <c r="L20">
         <v>1023.586</v>
       </c>
-      <c r="H20">
+      <c r="M20">
+        <v>2537.615</v>
+      </c>
+      <c r="N20">
         <v>1</v>
       </c>
-      <c r="I20">
+      <c r="O20">
         <v>1.597751931862364</v>
       </c>
-      <c r="J20">
+      <c r="P20">
         <v>1.833161356894105</v>
       </c>
-      <c r="K20">
+      <c r="Q20">
         <v>1.592074360035214</v>
       </c>
-      <c r="L20">
+      <c r="R20">
+        <v>1.18658663058569</v>
+      </c>
+      <c r="S20">
+        <v>0.8718557702688114</v>
+      </c>
+      <c r="T20">
+        <v>1.189319341791374</v>
+      </c>
+      <c r="U20">
         <v>41652230</v>
       </c>
-      <c r="M20">
+      <c r="V20">
         <v>1202513046</v>
       </c>
-      <c r="N20">
+      <c r="W20">
         <v>57.7406321822385</v>
       </c>
-      <c r="O20">
+      <c r="X20">
         <v>1892560</v>
       </c>
-      <c r="P20">
+      <c r="Y20">
         <v>519397580</v>
       </c>
-      <c r="Q20">
+      <c r="Z20">
         <v>39680179</v>
       </c>
-      <c r="R20">
+      <c r="AA20">
         <v>1200544694</v>
       </c>
-      <c r="S20">
+      <c r="AB20">
         <v>36.05133808510136</v>
       </c>
+      <c r="AC20">
+        <v>548.8836073889335</v>
+      </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:29">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B21">
         <v>1032.429</v>
@@ -1730,57 +2339,87 @@
         <v>25.867</v>
       </c>
       <c r="D21">
+        <v>872.9400000000001</v>
+      </c>
+      <c r="E21">
+        <v>37.256</v>
+      </c>
+      <c r="F21">
         <v>1006.562</v>
       </c>
-      <c r="E21">
+      <c r="G21">
+        <v>835.6840000000001</v>
+      </c>
+      <c r="H21">
         <v>1756.588</v>
       </c>
-      <c r="F21">
+      <c r="I21">
         <v>36.101</v>
       </c>
-      <c r="G21">
+      <c r="J21">
+        <v>937.3399999999999</v>
+      </c>
+      <c r="K21">
+        <v>35.29</v>
+      </c>
+      <c r="L21">
         <v>1720.487</v>
       </c>
-      <c r="H21">
+      <c r="M21">
+        <v>902.05</v>
+      </c>
+      <c r="N21">
         <v>1</v>
       </c>
-      <c r="I21">
+      <c r="O21">
         <v>1.701412881660627</v>
       </c>
-      <c r="J21">
+      <c r="P21">
         <v>1.395639231453203</v>
       </c>
-      <c r="K21">
+      <c r="Q21">
         <v>1.709270765238505</v>
       </c>
-      <c r="L21">
+      <c r="R21">
+        <v>1.073773684331111</v>
+      </c>
+      <c r="S21">
+        <v>0.9472299763796436</v>
+      </c>
+      <c r="T21">
+        <v>1.079415185644334</v>
+      </c>
+      <c r="U21">
         <v>65608366</v>
       </c>
-      <c r="M21">
+      <c r="V21">
         <v>1806067135</v>
       </c>
-      <c r="N21">
+      <c r="W21">
         <v>55.05600108986101</v>
       </c>
-      <c r="O21">
+      <c r="X21">
         <v>4258252</v>
       </c>
-      <c r="P21">
+      <c r="Y21">
         <v>636634507</v>
       </c>
-      <c r="Q21">
+      <c r="Z21">
         <v>51429670</v>
       </c>
-      <c r="R21">
+      <c r="AA21">
         <v>1791953648</v>
       </c>
-      <c r="S21">
+      <c r="AB21">
         <v>48.9838631096483</v>
       </c>
+      <c r="AC21">
+        <v>299.012133147592</v>
+      </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:29">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B22">
         <v>0.91</v>
@@ -1789,57 +2428,87 @@
         <v>0.123</v>
       </c>
       <c r="D22">
+        <v>0.073</v>
+      </c>
+      <c r="E22">
+        <v>0.051</v>
+      </c>
+      <c r="F22">
         <v>0.787</v>
       </c>
-      <c r="E22">
+      <c r="G22">
+        <v>0.022</v>
+      </c>
+      <c r="H22">
         <v>2.54</v>
       </c>
-      <c r="F22">
+      <c r="I22">
         <v>0.218</v>
       </c>
-      <c r="G22">
+      <c r="J22">
+        <v>0.311</v>
+      </c>
+      <c r="K22">
+        <v>0.035</v>
+      </c>
+      <c r="L22">
         <v>2.322</v>
       </c>
-      <c r="H22">
+      <c r="M22">
+        <v>0.276</v>
+      </c>
+      <c r="N22">
         <v>1</v>
       </c>
-      <c r="I22">
+      <c r="O22">
         <v>2.791208791208791</v>
       </c>
-      <c r="J22">
+      <c r="P22">
         <v>1.772357723577236</v>
       </c>
-      <c r="K22">
+      <c r="Q22">
         <v>2.950444726810673</v>
       </c>
-      <c r="L22">
+      <c r="R22">
+        <v>4.26027397260274</v>
+      </c>
+      <c r="S22">
+        <v>0.6862745098039216</v>
+      </c>
+      <c r="T22">
+        <v>12.54545454545455</v>
+      </c>
+      <c r="U22">
         <v>358937</v>
       </c>
-      <c r="M22">
+      <c r="V22">
         <v>2063645</v>
       </c>
-      <c r="N22">
+      <c r="W22">
         <v>11.49864739494675</v>
       </c>
-      <c r="O22">
+      <c r="X22">
         <v>333</v>
       </c>
-      <c r="P22">
+      <c r="Y22">
         <v>36473</v>
       </c>
-      <c r="Q22">
+      <c r="Z22">
         <v>218888</v>
       </c>
-      <c r="R22">
+      <c r="AA22">
         <v>1925411</v>
       </c>
-      <c r="S22">
+      <c r="AB22">
         <v>17.28569925190455</v>
       </c>
+      <c r="AC22">
+        <v>219.0570570570571</v>
+      </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:29">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B23">
         <v>2.041</v>
@@ -1848,57 +2517,87 @@
         <v>0.203</v>
       </c>
       <c r="D23">
+        <v>0.515</v>
+      </c>
+      <c r="E23">
+        <v>0.142</v>
+      </c>
+      <c r="F23">
         <v>1.838</v>
       </c>
-      <c r="E23">
+      <c r="G23">
+        <v>0.373</v>
+      </c>
+      <c r="H23">
         <v>5.774</v>
       </c>
-      <c r="F23">
+      <c r="I23">
         <v>0.291</v>
       </c>
-      <c r="G23">
+      <c r="J23">
+        <v>1.181</v>
+      </c>
+      <c r="K23">
+        <v>0.067</v>
+      </c>
+      <c r="L23">
         <v>5.483</v>
       </c>
-      <c r="H23">
+      <c r="M23">
+        <v>1.114</v>
+      </c>
+      <c r="N23">
         <v>1</v>
       </c>
-      <c r="I23">
+      <c r="O23">
         <v>2.829005389514944</v>
       </c>
-      <c r="J23">
+      <c r="P23">
         <v>1.433497536945813</v>
       </c>
-      <c r="K23">
+      <c r="Q23">
         <v>2.983133841131665</v>
       </c>
-      <c r="L23">
+      <c r="R23">
+        <v>2.293203883495146</v>
+      </c>
+      <c r="S23">
+        <v>0.4718309859154929</v>
+      </c>
+      <c r="T23">
+        <v>2.986595174262735</v>
+      </c>
+      <c r="U23">
         <v>456857</v>
       </c>
-      <c r="M23">
+      <c r="V23">
         <v>4081946</v>
       </c>
-      <c r="N23">
+      <c r="W23">
         <v>17.86968788920822</v>
       </c>
-      <c r="O23">
+      <c r="X23">
         <v>4868</v>
       </c>
-      <c r="P23">
+      <c r="Y23">
         <v>630874</v>
       </c>
-      <c r="Q23">
+      <c r="Z23">
         <v>308118</v>
       </c>
-      <c r="R23">
+      <c r="AA23">
         <v>3934188</v>
       </c>
-      <c r="S23">
+      <c r="AB23">
         <v>21.78607749381698</v>
       </c>
+      <c r="AC23">
+        <v>259.1922760887428</v>
+      </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:29">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B24">
         <v>4.728000000000001</v>
@@ -1907,57 +2606,87 @@
         <v>0.227</v>
       </c>
       <c r="D24">
+        <v>3.238</v>
+      </c>
+      <c r="E24">
+        <v>0.287</v>
+      </c>
+      <c r="F24">
         <v>4.501</v>
       </c>
-      <c r="E24">
+      <c r="G24">
+        <v>2.951</v>
+      </c>
+      <c r="H24">
         <v>11.562</v>
       </c>
-      <c r="F24">
+      <c r="I24">
         <v>0.333</v>
       </c>
-      <c r="G24">
+      <c r="J24">
+        <v>4.909</v>
+      </c>
+      <c r="K24">
+        <v>0.207</v>
+      </c>
+      <c r="L24">
         <v>11.229</v>
       </c>
-      <c r="H24">
+      <c r="M24">
+        <v>4.702</v>
+      </c>
+      <c r="N24">
         <v>1</v>
       </c>
-      <c r="I24">
+      <c r="O24">
         <v>2.445431472081218</v>
       </c>
-      <c r="J24">
+      <c r="P24">
         <v>1.466960352422908</v>
       </c>
-      <c r="K24">
+      <c r="Q24">
         <v>2.494778938013774</v>
       </c>
-      <c r="L24">
+      <c r="R24">
+        <v>1.516059295861643</v>
+      </c>
+      <c r="S24">
+        <v>0.7212543554006969</v>
+      </c>
+      <c r="T24">
+        <v>1.593358183666554</v>
+      </c>
+      <c r="U24">
         <v>559175</v>
       </c>
-      <c r="M24">
+      <c r="V24">
         <v>8029377</v>
       </c>
-      <c r="N24">
+      <c r="W24">
         <v>28.71865516162203</v>
       </c>
-      <c r="O24">
+      <c r="X24">
         <v>21068</v>
       </c>
-      <c r="P24">
+      <c r="Y24">
         <v>3145701</v>
       </c>
-      <c r="Q24">
+      <c r="Z24">
         <v>408682</v>
       </c>
-      <c r="R24">
+      <c r="AA24">
         <v>7879355</v>
       </c>
-      <c r="S24">
+      <c r="AB24">
         <v>24.42457702766154</v>
       </c>
+      <c r="AC24">
+        <v>298.6235997721663</v>
+      </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:29">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B25">
         <v>12.974</v>
@@ -1966,57 +2695,87 @@
         <v>0.296</v>
       </c>
       <c r="D25">
+        <v>14.365</v>
+      </c>
+      <c r="E25">
+        <v>0.467</v>
+      </c>
+      <c r="F25">
         <v>12.678</v>
       </c>
-      <c r="E25">
+      <c r="G25">
+        <v>13.898</v>
+      </c>
+      <c r="H25">
         <v>31.954</v>
       </c>
-      <c r="F25">
+      <c r="I25">
         <v>0.385</v>
       </c>
-      <c r="G25">
+      <c r="J25">
+        <v>19.096</v>
+      </c>
+      <c r="K25">
+        <v>0.37</v>
+      </c>
+      <c r="L25">
         <v>31.569</v>
       </c>
-      <c r="H25">
+      <c r="M25">
+        <v>18.726</v>
+      </c>
+      <c r="N25">
         <v>1</v>
       </c>
-      <c r="I25">
+      <c r="O25">
         <v>2.462925851703407</v>
       </c>
-      <c r="J25">
+      <c r="P25">
         <v>1.300675675675676</v>
       </c>
-      <c r="K25">
+      <c r="Q25">
         <v>2.490061523899669</v>
       </c>
-      <c r="L25">
+      <c r="R25">
+        <v>1.329342151061608</v>
+      </c>
+      <c r="S25">
+        <v>0.7922912205567452</v>
+      </c>
+      <c r="T25">
+        <v>1.347388113397611</v>
+      </c>
+      <c r="U25">
         <v>660444</v>
       </c>
-      <c r="M25">
+      <c r="V25">
         <v>15673919</v>
       </c>
-      <c r="N25">
+      <c r="W25">
         <v>47.4647933814222</v>
       </c>
-      <c r="O25">
+      <c r="X25">
         <v>40184</v>
       </c>
-      <c r="P25">
+      <c r="Y25">
         <v>7991992</v>
       </c>
-      <c r="Q25">
+      <c r="Z25">
         <v>517284</v>
       </c>
-      <c r="R25">
+      <c r="AA25">
         <v>15530946</v>
       </c>
-      <c r="S25">
+      <c r="AB25">
         <v>31.60324460280864</v>
       </c>
+      <c r="AC25">
+        <v>397.769858650209</v>
+      </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:29">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B26">
         <v>32.749</v>
@@ -2025,57 +2784,87 @@
         <v>0.388</v>
       </c>
       <c r="D26">
+        <v>57.76499999999999</v>
+      </c>
+      <c r="E26">
+        <v>0.695</v>
+      </c>
+      <c r="F26">
         <v>32.361</v>
       </c>
-      <c r="E26">
+      <c r="G26">
+        <v>57.06999999999999</v>
+      </c>
+      <c r="H26">
         <v>70.97399999999999</v>
       </c>
-      <c r="F26">
+      <c r="I26">
         <v>0.457</v>
       </c>
-      <c r="G26">
+      <c r="J26">
+        <v>74.321</v>
+      </c>
+      <c r="K26">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L26">
         <v>70.517</v>
       </c>
-      <c r="H26">
+      <c r="M26">
+        <v>73.773</v>
+      </c>
+      <c r="N26">
         <v>1</v>
       </c>
-      <c r="I26">
+      <c r="O26">
         <v>2.167211212556108</v>
       </c>
-      <c r="J26">
+      <c r="P26">
         <v>1.177835051546392</v>
       </c>
-      <c r="K26">
+      <c r="Q26">
         <v>2.179073576218287</v>
       </c>
-      <c r="L26">
+      <c r="R26">
+        <v>1.28660953864797</v>
+      </c>
+      <c r="S26">
+        <v>0.7884892086330935</v>
+      </c>
+      <c r="T26">
+        <v>1.292675661468372</v>
+      </c>
+      <c r="U26">
         <v>755026</v>
       </c>
-      <c r="M26">
+      <c r="V26">
         <v>30290104</v>
       </c>
-      <c r="N26">
+      <c r="W26">
         <v>80.23592300132711</v>
       </c>
-      <c r="O26">
+      <c r="X26">
         <v>60416</v>
       </c>
-      <c r="P26">
+      <c r="Y26">
         <v>18823438</v>
       </c>
-      <c r="Q26">
+      <c r="Z26">
         <v>626806</v>
       </c>
-      <c r="R26">
+      <c r="AA26">
         <v>30161953</v>
       </c>
-      <c r="S26">
+      <c r="AB26">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC26">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:29">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B27">
         <v>32.749</v>
@@ -2084,57 +2873,87 @@
         <v>0.388</v>
       </c>
       <c r="D27">
+        <v>57.76499999999999</v>
+      </c>
+      <c r="E27">
+        <v>0.695</v>
+      </c>
+      <c r="F27">
         <v>32.361</v>
       </c>
-      <c r="E27">
+      <c r="G27">
+        <v>57.06999999999999</v>
+      </c>
+      <c r="H27">
         <v>70.97399999999999</v>
       </c>
-      <c r="F27">
+      <c r="I27">
         <v>0.457</v>
       </c>
-      <c r="G27">
+      <c r="J27">
+        <v>74.321</v>
+      </c>
+      <c r="K27">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L27">
         <v>70.517</v>
       </c>
-      <c r="H27">
+      <c r="M27">
+        <v>73.773</v>
+      </c>
+      <c r="N27">
         <v>1</v>
       </c>
-      <c r="I27">
+      <c r="O27">
         <v>2.167211212556108</v>
       </c>
-      <c r="J27">
+      <c r="P27">
         <v>1.177835051546392</v>
       </c>
-      <c r="K27">
+      <c r="Q27">
         <v>2.179073576218287</v>
       </c>
-      <c r="L27">
+      <c r="R27">
+        <v>1.28660953864797</v>
+      </c>
+      <c r="S27">
+        <v>0.7884892086330935</v>
+      </c>
+      <c r="T27">
+        <v>1.292675661468372</v>
+      </c>
+      <c r="U27">
         <v>755026</v>
       </c>
-      <c r="M27">
+      <c r="V27">
         <v>30290104</v>
       </c>
-      <c r="N27">
+      <c r="W27">
         <v>80.23592300132711</v>
       </c>
-      <c r="O27">
+      <c r="X27">
         <v>60416</v>
       </c>
-      <c r="P27">
+      <c r="Y27">
         <v>18823438</v>
       </c>
-      <c r="Q27">
+      <c r="Z27">
         <v>626806</v>
       </c>
-      <c r="R27">
+      <c r="AA27">
         <v>30161953</v>
       </c>
-      <c r="S27">
+      <c r="AB27">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC27">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:29">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B28">
         <v>32.749</v>
@@ -2143,57 +2962,87 @@
         <v>0.388</v>
       </c>
       <c r="D28">
+        <v>57.76499999999999</v>
+      </c>
+      <c r="E28">
+        <v>0.695</v>
+      </c>
+      <c r="F28">
         <v>32.361</v>
       </c>
-      <c r="E28">
+      <c r="G28">
+        <v>57.06999999999999</v>
+      </c>
+      <c r="H28">
         <v>70.968</v>
       </c>
-      <c r="F28">
+      <c r="I28">
         <v>0.457</v>
       </c>
-      <c r="G28">
+      <c r="J28">
+        <v>74.333</v>
+      </c>
+      <c r="K28">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L28">
         <v>70.51100000000001</v>
       </c>
-      <c r="H28">
+      <c r="M28">
+        <v>73.785</v>
+      </c>
+      <c r="N28">
         <v>1</v>
       </c>
-      <c r="I28">
+      <c r="O28">
         <v>2.167028000854988</v>
       </c>
-      <c r="J28">
+      <c r="P28">
         <v>1.177835051546392</v>
       </c>
-      <c r="K28">
+      <c r="Q28">
         <v>2.17888816785637</v>
       </c>
-      <c r="L28">
+      <c r="R28">
+        <v>1.286817276897776</v>
+      </c>
+      <c r="S28">
+        <v>0.7884892086330935</v>
+      </c>
+      <c r="T28">
+        <v>1.292885929560189</v>
+      </c>
+      <c r="U28">
         <v>755026</v>
       </c>
-      <c r="M28">
+      <c r="V28">
         <v>30290104</v>
       </c>
-      <c r="N28">
+      <c r="W28">
         <v>80.23592300132711</v>
       </c>
-      <c r="O28">
+      <c r="X28">
         <v>60416</v>
       </c>
-      <c r="P28">
+      <c r="Y28">
         <v>18823438</v>
       </c>
-      <c r="Q28">
+      <c r="Z28">
         <v>626806</v>
       </c>
-      <c r="R28">
+      <c r="AA28">
         <v>30161953</v>
       </c>
-      <c r="S28">
+      <c r="AB28">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC28">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:29">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B29">
         <v>32.749</v>
@@ -2202,57 +3051,87 @@
         <v>0.388</v>
       </c>
       <c r="D29">
+        <v>57.76499999999999</v>
+      </c>
+      <c r="E29">
+        <v>0.695</v>
+      </c>
+      <c r="F29">
         <v>32.361</v>
       </c>
-      <c r="E29">
+      <c r="G29">
+        <v>57.06999999999999</v>
+      </c>
+      <c r="H29">
         <v>70.968</v>
       </c>
-      <c r="F29">
+      <c r="I29">
         <v>0.457</v>
       </c>
-      <c r="G29">
+      <c r="J29">
+        <v>74.333</v>
+      </c>
+      <c r="K29">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L29">
         <v>70.51100000000001</v>
       </c>
-      <c r="H29">
+      <c r="M29">
+        <v>73.785</v>
+      </c>
+      <c r="N29">
         <v>1</v>
       </c>
-      <c r="I29">
+      <c r="O29">
         <v>2.167028000854988</v>
       </c>
-      <c r="J29">
+      <c r="P29">
         <v>1.177835051546392</v>
       </c>
-      <c r="K29">
+      <c r="Q29">
         <v>2.17888816785637</v>
       </c>
-      <c r="L29">
+      <c r="R29">
+        <v>1.286817276897776</v>
+      </c>
+      <c r="S29">
+        <v>0.7884892086330935</v>
+      </c>
+      <c r="T29">
+        <v>1.292885929560189</v>
+      </c>
+      <c r="U29">
         <v>755026</v>
       </c>
-      <c r="M29">
+      <c r="V29">
         <v>30290104</v>
       </c>
-      <c r="N29">
+      <c r="W29">
         <v>80.23592300132711</v>
       </c>
-      <c r="O29">
+      <c r="X29">
         <v>60416</v>
       </c>
-      <c r="P29">
+      <c r="Y29">
         <v>18823438</v>
       </c>
-      <c r="Q29">
+      <c r="Z29">
         <v>626806</v>
       </c>
-      <c r="R29">
+      <c r="AA29">
         <v>30161953</v>
       </c>
-      <c r="S29">
+      <c r="AB29">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC29">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:29">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B30">
         <v>51.838</v>
@@ -2261,57 +3140,87 @@
         <v>0.378</v>
       </c>
       <c r="D30">
+        <v>236.095</v>
+      </c>
+      <c r="E30">
+        <v>1.491</v>
+      </c>
+      <c r="F30">
         <v>51.46</v>
       </c>
-      <c r="E30">
+      <c r="G30">
+        <v>234.604</v>
+      </c>
+      <c r="H30">
         <v>100.09</v>
       </c>
-      <c r="F30">
+      <c r="I30">
         <v>0.473</v>
       </c>
-      <c r="G30">
+      <c r="J30">
+        <v>294.236</v>
+      </c>
+      <c r="K30">
+        <v>1.223</v>
+      </c>
+      <c r="L30">
         <v>99.617</v>
       </c>
-      <c r="H30">
+      <c r="M30">
+        <v>293.013</v>
+      </c>
+      <c r="N30">
         <v>1</v>
       </c>
-      <c r="I30">
+      <c r="O30">
         <v>1.93082294841622</v>
       </c>
-      <c r="J30">
+      <c r="P30">
         <v>1.251322751322751</v>
       </c>
-      <c r="K30">
+      <c r="Q30">
         <v>1.935814224640497</v>
       </c>
-      <c r="L30">
+      <c r="R30">
+        <v>1.246261038988543</v>
+      </c>
+      <c r="S30">
+        <v>0.8202548625083836</v>
+      </c>
+      <c r="T30">
+        <v>1.248968474535814</v>
+      </c>
+      <c r="U30">
         <v>837036</v>
       </c>
-      <c r="M30">
+      <c r="V30">
         <v>57814555</v>
       </c>
-      <c r="N30">
+      <c r="W30">
         <v>138.1411432722129</v>
       </c>
-      <c r="O30">
+      <c r="X30">
         <v>137879</v>
       </c>
-      <c r="P30">
+      <c r="Y30">
         <v>46629291</v>
       </c>
-      <c r="Q30">
+      <c r="Z30">
         <v>728771</v>
       </c>
-      <c r="R30">
+      <c r="AA30">
         <v>57706306</v>
       </c>
-      <c r="S30">
+      <c r="AB30">
         <v>37.49251978364913</v>
       </c>
+      <c r="AC30">
+        <v>676.3798838111678</v>
+      </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:29">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B31">
         <v>91.75800000000001</v>
@@ -2320,57 +3229,87 @@
         <v>0.41</v>
       </c>
       <c r="D31">
+        <v>785.628</v>
+      </c>
+      <c r="E31">
+        <v>2.618</v>
+      </c>
+      <c r="F31">
         <v>91.34800000000001</v>
       </c>
-      <c r="E31">
+      <c r="G31">
+        <v>783.01</v>
+      </c>
+      <c r="H31">
         <v>186.373</v>
       </c>
-      <c r="F31">
+      <c r="I31">
         <v>0.481</v>
       </c>
-      <c r="G31">
+      <c r="J31">
+        <v>980.401</v>
+      </c>
+      <c r="K31">
+        <v>2.09</v>
+      </c>
+      <c r="L31">
         <v>185.892</v>
       </c>
-      <c r="H31">
+      <c r="M31">
+        <v>978.3109999999999</v>
+      </c>
+      <c r="N31">
         <v>1</v>
       </c>
-      <c r="I31">
+      <c r="O31">
         <v>2.031136249700299</v>
       </c>
-      <c r="J31">
+      <c r="P31">
         <v>1.173170731707317</v>
       </c>
-      <c r="K31">
+      <c r="Q31">
         <v>2.034987082366335</v>
       </c>
-      <c r="L31">
+      <c r="R31">
+        <v>1.247920135229396</v>
+      </c>
+      <c r="S31">
+        <v>0.7983193277310924</v>
+      </c>
+      <c r="T31">
+        <v>1.249423379011762</v>
+      </c>
+      <c r="U31">
         <v>904525</v>
       </c>
-      <c r="M31">
+      <c r="V31">
         <v>108747344</v>
       </c>
-      <c r="N31">
+      <c r="W31">
         <v>240.45182609657</v>
       </c>
-      <c r="O31">
+      <c r="X31">
         <v>228316</v>
       </c>
-      <c r="P31">
+      <c r="Y31">
         <v>96371407</v>
       </c>
-      <c r="Q31">
+      <c r="Z31">
         <v>819137</v>
       </c>
-      <c r="R31">
+      <c r="AA31">
         <v>108661967</v>
       </c>
-      <c r="S31">
+      <c r="AB31">
         <v>41.60502081002537</v>
       </c>
+      <c r="AC31">
+        <v>844.1931971478127</v>
+      </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:29">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B32">
         <v>207.622</v>
@@ -2379,57 +3318,87 @@
         <v>0.53</v>
       </c>
       <c r="D32">
+        <v>2420.24</v>
+      </c>
+      <c r="E32">
+        <v>3.85</v>
+      </c>
+      <c r="F32">
         <v>207.092</v>
       </c>
-      <c r="E32">
+      <c r="G32">
+        <v>2416.39</v>
+      </c>
+      <c r="H32">
         <v>393.392</v>
       </c>
-      <c r="F32">
+      <c r="I32">
         <v>0.521</v>
       </c>
-      <c r="G32">
+      <c r="J32">
+        <v>3061.045</v>
+      </c>
+      <c r="K32">
+        <v>2.841</v>
+      </c>
+      <c r="L32">
         <v>392.871</v>
       </c>
-      <c r="H32">
+      <c r="M32">
+        <v>3058.204</v>
+      </c>
+      <c r="N32">
         <v>1</v>
       </c>
-      <c r="I32">
+      <c r="O32">
         <v>1.894751037943956</v>
       </c>
-      <c r="J32">
+      <c r="P32">
         <v>0.9830188679245283</v>
       </c>
-      <c r="K32">
+      <c r="Q32">
         <v>1.897084387615166</v>
       </c>
-      <c r="L32">
+      <c r="R32">
+        <v>1.264769196443328</v>
+      </c>
+      <c r="S32">
+        <v>0.737922077922078</v>
+      </c>
+      <c r="T32">
+        <v>1.265608614503453</v>
+      </c>
+      <c r="U32">
         <v>955990</v>
       </c>
-      <c r="M32">
+      <c r="V32">
         <v>201086863</v>
       </c>
-      <c r="N32">
+      <c r="W32">
         <v>420.6882143118652</v>
       </c>
-      <c r="O32">
+      <c r="X32">
         <v>263944</v>
       </c>
-      <c r="P32">
+      <c r="Y32">
         <v>183139066</v>
       </c>
-      <c r="Q32">
+      <c r="Z32">
         <v>892588</v>
       </c>
-      <c r="R32">
+      <c r="AA32">
         <v>201023463</v>
       </c>
-      <c r="S32">
+      <c r="AB32">
         <v>56.89833037458403</v>
       </c>
+      <c r="AC32">
+        <v>1387.711529718425</v>
+      </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:29">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B33">
         <v>1.891</v>
@@ -2438,57 +3407,87 @@
         <v>0.148</v>
       </c>
       <c r="D33">
+        <v>2.004</v>
+      </c>
+      <c r="E33">
+        <v>0.187</v>
+      </c>
+      <c r="F33">
         <v>1.743</v>
       </c>
-      <c r="E33">
+      <c r="G33">
+        <v>1.817</v>
+      </c>
+      <c r="H33">
         <v>7.715</v>
       </c>
-      <c r="F33">
+      <c r="I33">
         <v>0.08399999999999999</v>
       </c>
-      <c r="G33">
+      <c r="J33">
+        <v>3.712</v>
+      </c>
+      <c r="K33">
+        <v>0.111</v>
+      </c>
+      <c r="L33">
         <v>7.631</v>
       </c>
-      <c r="H33">
+      <c r="M33">
+        <v>3.601</v>
+      </c>
+      <c r="N33">
         <v>1</v>
       </c>
-      <c r="I33">
+      <c r="O33">
         <v>4.079851930195663</v>
       </c>
-      <c r="J33">
+      <c r="P33">
         <v>0.5675675675675675</v>
       </c>
-      <c r="K33">
+      <c r="Q33">
         <v>4.378083763625932</v>
       </c>
-      <c r="L33">
+      <c r="R33">
+        <v>1.852295409181637</v>
+      </c>
+      <c r="S33">
+        <v>0.5935828877005348</v>
+      </c>
+      <c r="T33">
+        <v>1.981838194826637</v>
+      </c>
+      <c r="U33">
         <v>102869</v>
       </c>
-      <c r="M33">
+      <c r="V33">
         <v>3521310</v>
       </c>
-      <c r="N33">
+      <c r="W33">
         <v>68.46202451661823</v>
       </c>
-      <c r="O33">
+      <c r="X33">
         <v>9301</v>
       </c>
-      <c r="P33">
+      <c r="Y33">
         <v>1961680</v>
       </c>
-      <c r="Q33">
+      <c r="Z33">
         <v>87794</v>
       </c>
-      <c r="R33">
+      <c r="AA33">
         <v>3506244</v>
       </c>
-      <c r="S33">
+      <c r="AB33">
         <v>39.35545844852408</v>
       </c>
+      <c r="AC33">
+        <v>421.821309536609</v>
+      </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:29">
       <c r="A34" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B34">
         <v>5.34</v>
@@ -2497,57 +3496,87 @@
         <v>0.195</v>
       </c>
       <c r="D34">
+        <v>6.021</v>
+      </c>
+      <c r="E34">
+        <v>0.256</v>
+      </c>
+      <c r="F34">
         <v>5.145</v>
       </c>
-      <c r="E34">
+      <c r="G34">
+        <v>5.765</v>
+      </c>
+      <c r="H34">
         <v>18.753</v>
       </c>
-      <c r="F34">
+      <c r="I34">
         <v>0.144</v>
       </c>
-      <c r="G34">
+      <c r="J34">
+        <v>9.195</v>
+      </c>
+      <c r="K34">
+        <v>0.173</v>
+      </c>
+      <c r="L34">
         <v>18.609</v>
       </c>
-      <c r="H34">
+      <c r="M34">
+        <v>9.022</v>
+      </c>
+      <c r="N34">
         <v>1</v>
       </c>
-      <c r="I34">
+      <c r="O34">
         <v>3.511797752808989</v>
       </c>
-      <c r="J34">
+      <c r="P34">
         <v>0.7384615384615385</v>
       </c>
-      <c r="K34">
+      <c r="Q34">
         <v>3.616909620991254</v>
       </c>
-      <c r="L34">
+      <c r="R34">
+        <v>1.527154957648231</v>
+      </c>
+      <c r="S34">
+        <v>0.67578125</v>
+      </c>
+      <c r="T34">
+        <v>1.564960971379011</v>
+      </c>
+      <c r="U34">
         <v>199881</v>
       </c>
-      <c r="M34">
+      <c r="V34">
         <v>7248722</v>
       </c>
-      <c r="N34">
+      <c r="W34">
         <v>72.53037557346622</v>
       </c>
-      <c r="O34">
+      <c r="X34">
         <v>16521</v>
       </c>
-      <c r="P34">
+      <c r="Y34">
         <v>3979866</v>
       </c>
-      <c r="Q34">
+      <c r="Z34">
         <v>169152</v>
       </c>
-      <c r="R34">
+      <c r="AA34">
         <v>7218010</v>
       </c>
-      <c r="S34">
+      <c r="AB34">
         <v>42.43101335901619</v>
       </c>
+      <c r="AC34">
+        <v>481.7948066097694</v>
+      </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:29">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B35">
         <v>10.114</v>
@@ -2556,57 +3585,87 @@
         <v>0.226</v>
       </c>
       <c r="D35">
+        <v>22.528</v>
+      </c>
+      <c r="E35">
+        <v>0.508</v>
+      </c>
+      <c r="F35">
         <v>9.887999999999998</v>
       </c>
-      <c r="E35">
+      <c r="G35">
+        <v>22.02</v>
+      </c>
+      <c r="H35">
         <v>23.511</v>
       </c>
-      <c r="F35">
+      <c r="I35">
         <v>0.237</v>
       </c>
-      <c r="G35">
+      <c r="J35">
+        <v>29.934</v>
+      </c>
+      <c r="K35">
+        <v>0.4</v>
+      </c>
+      <c r="L35">
         <v>23.274</v>
       </c>
-      <c r="H35">
+      <c r="M35">
+        <v>29.534</v>
+      </c>
+      <c r="N35">
         <v>1</v>
       </c>
-      <c r="I35">
+      <c r="O35">
         <v>2.324599564959462</v>
       </c>
-      <c r="J35">
+      <c r="P35">
         <v>1.048672566371681</v>
       </c>
-      <c r="K35">
+      <c r="Q35">
         <v>2.353762135922331</v>
       </c>
-      <c r="L35">
+      <c r="R35">
+        <v>1.328746448863636</v>
+      </c>
+      <c r="S35">
+        <v>0.7874015748031497</v>
+      </c>
+      <c r="T35">
+        <v>1.341235240690281</v>
+      </c>
+      <c r="U35">
         <v>388707</v>
       </c>
-      <c r="M35">
+      <c r="V35">
         <v>14843582</v>
       </c>
-      <c r="N35">
+      <c r="W35">
         <v>76.37414299202227</v>
       </c>
-      <c r="O35">
+      <c r="X35">
         <v>43695</v>
       </c>
-      <c r="P35">
+      <c r="Y35">
         <v>10105463</v>
       </c>
-      <c r="Q35">
+      <c r="Z35">
         <v>325306</v>
       </c>
-      <c r="R35">
+      <c r="AA35">
         <v>14780230</v>
       </c>
-      <c r="S35">
+      <c r="AB35">
         <v>33.20017328868546</v>
       </c>
+      <c r="AC35">
+        <v>462.5455086394325</v>
+      </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:29">
       <c r="A36" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B36">
         <v>32.752</v>
@@ -2615,57 +3674,87 @@
         <v>0.389</v>
       </c>
       <c r="D36">
+        <v>57.812</v>
+      </c>
+      <c r="E36">
+        <v>0.6920000000000001</v>
+      </c>
+      <c r="F36">
         <v>32.363</v>
       </c>
-      <c r="E36">
+      <c r="G36">
+        <v>57.12</v>
+      </c>
+      <c r="H36">
         <v>70.97399999999999</v>
       </c>
-      <c r="F36">
+      <c r="I36">
         <v>0.457</v>
       </c>
-      <c r="G36">
+      <c r="J36">
+        <v>74.321</v>
+      </c>
+      <c r="K36">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L36">
         <v>70.517</v>
       </c>
-      <c r="H36">
+      <c r="M36">
+        <v>73.773</v>
+      </c>
+      <c r="N36">
         <v>1</v>
       </c>
-      <c r="I36">
+      <c r="O36">
         <v>2.167012701514411</v>
       </c>
-      <c r="J36">
+      <c r="P36">
         <v>1.174807197943445</v>
       </c>
-      <c r="K36">
+      <c r="Q36">
         <v>2.178938911720174</v>
       </c>
-      <c r="L36">
+      <c r="R36">
+        <v>1.285563550819899</v>
+      </c>
+      <c r="S36">
+        <v>0.7919075144508669</v>
+      </c>
+      <c r="T36">
+        <v>1.291544117647059</v>
+      </c>
+      <c r="U36">
         <v>755026</v>
       </c>
-      <c r="M36">
+      <c r="V36">
         <v>30290104</v>
       </c>
-      <c r="N36">
+      <c r="W36">
         <v>80.23592300132711</v>
       </c>
-      <c r="O36">
+      <c r="X36">
         <v>60416</v>
       </c>
-      <c r="P36">
+      <c r="Y36">
         <v>18823438</v>
       </c>
-      <c r="Q36">
+      <c r="Z36">
         <v>626806</v>
       </c>
-      <c r="R36">
+      <c r="AA36">
         <v>30161953</v>
       </c>
-      <c r="S36">
+      <c r="AB36">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC36">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:29">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B37">
         <v>32.752</v>
@@ -2674,57 +3763,87 @@
         <v>0.389</v>
       </c>
       <c r="D37">
+        <v>57.812</v>
+      </c>
+      <c r="E37">
+        <v>0.6920000000000001</v>
+      </c>
+      <c r="F37">
         <v>32.363</v>
       </c>
-      <c r="E37">
+      <c r="G37">
+        <v>57.12</v>
+      </c>
+      <c r="H37">
         <v>70.97399999999999</v>
       </c>
-      <c r="F37">
+      <c r="I37">
         <v>0.457</v>
       </c>
-      <c r="G37">
+      <c r="J37">
+        <v>74.321</v>
+      </c>
+      <c r="K37">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L37">
         <v>70.517</v>
       </c>
-      <c r="H37">
+      <c r="M37">
+        <v>73.773</v>
+      </c>
+      <c r="N37">
         <v>1</v>
       </c>
-      <c r="I37">
+      <c r="O37">
         <v>2.167012701514411</v>
       </c>
-      <c r="J37">
+      <c r="P37">
         <v>1.174807197943445</v>
       </c>
-      <c r="K37">
+      <c r="Q37">
         <v>2.178938911720174</v>
       </c>
-      <c r="L37">
+      <c r="R37">
+        <v>1.285563550819899</v>
+      </c>
+      <c r="S37">
+        <v>0.7919075144508669</v>
+      </c>
+      <c r="T37">
+        <v>1.291544117647059</v>
+      </c>
+      <c r="U37">
         <v>755026</v>
       </c>
-      <c r="M37">
+      <c r="V37">
         <v>30290104</v>
       </c>
-      <c r="N37">
+      <c r="W37">
         <v>80.23592300132711</v>
       </c>
-      <c r="O37">
+      <c r="X37">
         <v>60416</v>
       </c>
-      <c r="P37">
+      <c r="Y37">
         <v>18823438</v>
       </c>
-      <c r="Q37">
+      <c r="Z37">
         <v>626806</v>
       </c>
-      <c r="R37">
+      <c r="AA37">
         <v>30161953</v>
       </c>
-      <c r="S37">
+      <c r="AB37">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC37">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:29">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B38">
         <v>32.752</v>
@@ -2733,57 +3852,87 @@
         <v>0.389</v>
       </c>
       <c r="D38">
+        <v>57.812</v>
+      </c>
+      <c r="E38">
+        <v>0.6920000000000001</v>
+      </c>
+      <c r="F38">
         <v>32.363</v>
       </c>
-      <c r="E38">
+      <c r="G38">
+        <v>57.12</v>
+      </c>
+      <c r="H38">
         <v>70.968</v>
       </c>
-      <c r="F38">
+      <c r="I38">
         <v>0.457</v>
       </c>
-      <c r="G38">
+      <c r="J38">
+        <v>74.333</v>
+      </c>
+      <c r="K38">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L38">
         <v>70.51100000000001</v>
       </c>
-      <c r="H38">
+      <c r="M38">
+        <v>73.785</v>
+      </c>
+      <c r="N38">
         <v>1</v>
       </c>
-      <c r="I38">
+      <c r="O38">
         <v>2.166829506595017</v>
       </c>
-      <c r="J38">
+      <c r="P38">
         <v>1.174807197943445</v>
       </c>
-      <c r="K38">
+      <c r="Q38">
         <v>2.178753514816303</v>
       </c>
-      <c r="L38">
+      <c r="R38">
+        <v>1.285771120182661</v>
+      </c>
+      <c r="S38">
+        <v>0.7919075144508669</v>
+      </c>
+      <c r="T38">
+        <v>1.291754201680672</v>
+      </c>
+      <c r="U38">
         <v>755026</v>
       </c>
-      <c r="M38">
+      <c r="V38">
         <v>30290104</v>
       </c>
-      <c r="N38">
+      <c r="W38">
         <v>80.23592300132711</v>
       </c>
-      <c r="O38">
+      <c r="X38">
         <v>60416</v>
       </c>
-      <c r="P38">
+      <c r="Y38">
         <v>18823438</v>
       </c>
-      <c r="Q38">
+      <c r="Z38">
         <v>626806</v>
       </c>
-      <c r="R38">
+      <c r="AA38">
         <v>30161953</v>
       </c>
-      <c r="S38">
+      <c r="AB38">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC38">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:29">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B39">
         <v>32.752</v>
@@ -2792,57 +3941,87 @@
         <v>0.389</v>
       </c>
       <c r="D39">
+        <v>57.812</v>
+      </c>
+      <c r="E39">
+        <v>0.6920000000000001</v>
+      </c>
+      <c r="F39">
         <v>32.363</v>
       </c>
-      <c r="E39">
+      <c r="G39">
+        <v>57.12</v>
+      </c>
+      <c r="H39">
         <v>70.968</v>
       </c>
-      <c r="F39">
+      <c r="I39">
         <v>0.457</v>
       </c>
-      <c r="G39">
+      <c r="J39">
+        <v>74.333</v>
+      </c>
+      <c r="K39">
+        <v>0.5479999999999999</v>
+      </c>
+      <c r="L39">
         <v>70.51100000000001</v>
       </c>
-      <c r="H39">
+      <c r="M39">
+        <v>73.785</v>
+      </c>
+      <c r="N39">
         <v>1</v>
       </c>
-      <c r="I39">
+      <c r="O39">
         <v>2.166829506595017</v>
       </c>
-      <c r="J39">
+      <c r="P39">
         <v>1.174807197943445</v>
       </c>
-      <c r="K39">
+      <c r="Q39">
         <v>2.178753514816303</v>
       </c>
-      <c r="L39">
+      <c r="R39">
+        <v>1.285771120182661</v>
+      </c>
+      <c r="S39">
+        <v>0.7919075144508669</v>
+      </c>
+      <c r="T39">
+        <v>1.291754201680672</v>
+      </c>
+      <c r="U39">
         <v>755026</v>
       </c>
-      <c r="M39">
+      <c r="V39">
         <v>30290104</v>
       </c>
-      <c r="N39">
+      <c r="W39">
         <v>80.23592300132711</v>
       </c>
-      <c r="O39">
+      <c r="X39">
         <v>60416</v>
       </c>
-      <c r="P39">
+      <c r="Y39">
         <v>18823438</v>
       </c>
-      <c r="Q39">
+      <c r="Z39">
         <v>626806</v>
       </c>
-      <c r="R39">
+      <c r="AA39">
         <v>30161953</v>
       </c>
-      <c r="S39">
+      <c r="AB39">
         <v>40.03783611998799</v>
       </c>
+      <c r="AC39">
+        <v>623.1275820974577</v>
+      </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:29">
       <c r="A40" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B40">
         <v>54.532</v>
@@ -2851,57 +4030,87 @@
         <v>0.465</v>
       </c>
       <c r="D40">
+        <v>193.099</v>
+      </c>
+      <c r="E40">
+        <v>1.896</v>
+      </c>
+      <c r="F40">
         <v>54.06699999999999</v>
       </c>
-      <c r="E40">
+      <c r="G40">
+        <v>191.203</v>
+      </c>
+      <c r="H40">
         <v>101.223</v>
       </c>
-      <c r="F40">
+      <c r="I40">
         <v>0.784</v>
       </c>
-      <c r="G40">
+      <c r="J40">
+        <v>234.274</v>
+      </c>
+      <c r="K40">
+        <v>1.636</v>
+      </c>
+      <c r="L40">
         <v>100.439</v>
       </c>
-      <c r="H40">
+      <c r="M40">
+        <v>232.638</v>
+      </c>
+      <c r="N40">
         <v>1</v>
       </c>
-      <c r="I40">
+      <c r="O40">
         <v>1.856212865840241</v>
       </c>
-      <c r="J40">
+      <c r="P40">
         <v>1.686021505376344</v>
       </c>
-      <c r="K40">
+      <c r="Q40">
         <v>1.857676586457544</v>
       </c>
-      <c r="L40">
+      <c r="R40">
+        <v>1.213232590536461</v>
+      </c>
+      <c r="S40">
+        <v>0.8628691983122364</v>
+      </c>
+      <c r="T40">
+        <v>1.21670685083393</v>
+      </c>
+      <c r="U40">
         <v>1465546</v>
       </c>
-      <c r="M40">
+      <c r="V40">
         <v>61604169</v>
       </c>
-      <c r="N40">
+      <c r="W40">
         <v>84.06992206317645</v>
       </c>
-      <c r="O40">
+      <c r="X40">
         <v>189948</v>
       </c>
-      <c r="P40">
+      <c r="Y40">
         <v>46571394</v>
       </c>
-      <c r="Q40">
+      <c r="Z40">
         <v>1204507</v>
       </c>
-      <c r="R40">
+      <c r="AA40">
         <v>61343269</v>
       </c>
-      <c r="S40">
+      <c r="AB40">
         <v>29.11979490596407</v>
       </c>
+      <c r="AC40">
+        <v>490.3594036262556</v>
+      </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:29">
       <c r="A41" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B41">
         <v>164.537</v>
@@ -2910,57 +4119,87 @@
         <v>0.907</v>
       </c>
       <c r="D41">
+        <v>489.734</v>
+      </c>
+      <c r="E41">
+        <v>2.897</v>
+      </c>
+      <c r="F41">
         <v>163.63</v>
       </c>
-      <c r="E41">
+      <c r="G41">
+        <v>486.837</v>
+      </c>
+      <c r="H41">
         <v>290.896</v>
       </c>
-      <c r="F41">
+      <c r="I41">
         <v>1.555</v>
       </c>
-      <c r="G41">
+      <c r="J41">
+        <v>589.3150000000001</v>
+      </c>
+      <c r="K41">
+        <v>2.442</v>
+      </c>
+      <c r="L41">
         <v>289.341</v>
       </c>
-      <c r="H41">
+      <c r="M41">
+        <v>586.873</v>
+      </c>
+      <c r="N41">
         <v>1</v>
       </c>
-      <c r="I41">
+      <c r="O41">
         <v>1.767967083391578</v>
       </c>
-      <c r="J41">
+      <c r="P41">
         <v>1.714443219404631</v>
       </c>
-      <c r="K41">
+      <c r="Q41">
         <v>1.768263765813115</v>
       </c>
-      <c r="L41">
+      <c r="R41">
+        <v>1.20333691350815</v>
+      </c>
+      <c r="S41">
+        <v>0.8429409734207802</v>
+      </c>
+      <c r="T41">
+        <v>1.205481506130389</v>
+      </c>
+      <c r="U41">
         <v>2845797</v>
       </c>
-      <c r="M41">
+      <c r="V41">
         <v>124942349</v>
       </c>
-      <c r="N41">
+      <c r="W41">
         <v>87.80833559104883</v>
       </c>
-      <c r="O41">
+      <c r="X41">
         <v>280499</v>
       </c>
-      <c r="P41">
+      <c r="Y41">
         <v>89862334</v>
       </c>
-      <c r="Q41">
+      <c r="Z41">
         <v>2315813</v>
       </c>
-      <c r="R41">
+      <c r="AA41">
         <v>124412652</v>
       </c>
-      <c r="S41">
+      <c r="AB41">
         <v>33.95084787900049</v>
       </c>
+      <c r="AC41">
+        <v>640.7319384382832</v>
+      </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:29">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B42">
         <v>501.3680000000001</v>
@@ -2969,57 +4208,87 @@
         <v>1.959</v>
       </c>
       <c r="D42">
+        <v>1210.892</v>
+      </c>
+      <c r="E42">
+        <v>4.505999999999999</v>
+      </c>
+      <c r="F42">
         <v>499.409</v>
       </c>
-      <c r="E42">
+      <c r="G42">
+        <v>1206.386</v>
+      </c>
+      <c r="H42">
         <v>899</v>
       </c>
-      <c r="F42">
+      <c r="I42">
         <v>3.101</v>
       </c>
-      <c r="G42">
+      <c r="J42">
+        <v>1461.636</v>
+      </c>
+      <c r="K42">
+        <v>3.637</v>
+      </c>
+      <c r="L42">
         <v>895.899</v>
       </c>
-      <c r="H42">
+      <c r="M42">
+        <v>1457.999</v>
+      </c>
+      <c r="N42">
         <v>1</v>
       </c>
-      <c r="I42">
+      <c r="O42">
         <v>1.793094094557291</v>
       </c>
-      <c r="J42">
+      <c r="P42">
         <v>1.582950484941297</v>
       </c>
-      <c r="K42">
+      <c r="Q42">
         <v>1.793918411562467</v>
       </c>
-      <c r="L42">
+      <c r="R42">
+        <v>1.207073793534023</v>
+      </c>
+      <c r="S42">
+        <v>0.8071460275188639</v>
+      </c>
+      <c r="T42">
+        <v>1.208567572899553</v>
+      </c>
+      <c r="U42">
         <v>5520326</v>
       </c>
-      <c r="M42">
+      <c r="V42">
         <v>252819809</v>
       </c>
-      <c r="N42">
+      <c r="W42">
         <v>91.59597060028702</v>
       </c>
-      <c r="O42">
+      <c r="X42">
         <v>403463</v>
       </c>
-      <c r="P42">
+      <c r="Y42">
         <v>169764840</v>
       </c>
-      <c r="Q42">
+      <c r="Z42">
         <v>4460152</v>
       </c>
-      <c r="R42">
+      <c r="AA42">
         <v>251760234</v>
       </c>
-      <c r="S42">
+      <c r="AB42">
         <v>40.42478681506027</v>
       </c>
+      <c r="AC42">
+        <v>841.5385797458503</v>
+      </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:29">
       <c r="A43" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B43">
         <v>787.883</v>
@@ -3028,52 +4297,82 @@
         <v>2.458</v>
       </c>
       <c r="D43">
+        <v>3643.182</v>
+      </c>
+      <c r="E43">
+        <v>12.876</v>
+      </c>
+      <c r="F43">
         <v>785.4250000000001</v>
       </c>
-      <c r="E43">
+      <c r="G43">
+        <v>3630.306</v>
+      </c>
+      <c r="H43">
         <v>1270.524</v>
       </c>
-      <c r="F43">
+      <c r="I43">
         <v>5.471</v>
       </c>
-      <c r="G43">
+      <c r="J43">
+        <v>4347.868</v>
+      </c>
+      <c r="K43">
+        <v>11.024</v>
+      </c>
+      <c r="L43">
         <v>1265.053</v>
       </c>
-      <c r="H43">
+      <c r="M43">
+        <v>4336.844</v>
+      </c>
+      <c r="N43">
         <v>1</v>
       </c>
-      <c r="I43">
+      <c r="O43">
         <v>1.612579532747882</v>
       </c>
-      <c r="J43">
+      <c r="P43">
         <v>2.225793327908869</v>
       </c>
-      <c r="K43">
+      <c r="Q43">
         <v>1.610660470445937</v>
       </c>
-      <c r="L43">
+      <c r="R43">
+        <v>1.193425966641249</v>
+      </c>
+      <c r="S43">
+        <v>0.8561665113389252</v>
+      </c>
+      <c r="T43">
+        <v>1.194622161327447</v>
+      </c>
+      <c r="U43">
         <v>10708196</v>
       </c>
-      <c r="M43">
+      <c r="V43">
         <v>510588330</v>
       </c>
-      <c r="N43">
+      <c r="W43">
         <v>95.36402396818288</v>
       </c>
-      <c r="O43">
+      <c r="X43">
         <v>1269873</v>
       </c>
-      <c r="P43">
+      <c r="Y43">
         <v>404162374</v>
       </c>
-      <c r="Q43">
+      <c r="Z43">
         <v>8578357</v>
       </c>
-      <c r="R43">
+      <c r="AA43">
         <v>508459676</v>
       </c>
-      <c r="S43">
+      <c r="AB43">
         <v>28.5414326692102</v>
+      </c>
+      <c r="AC43">
+        <v>636.5398335109102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix error data of grouptc-cuckoo
</commit_message>
<xml_diff>
--- a/excel/grouptc_hs_vs_trust_time.xlsx
+++ b/excel/grouptc_hs_vs_trust_time.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Datasets</t>
   </si>
@@ -672,16 +672,16 @@
         <v>0.092</v>
       </c>
       <c r="D2">
-        <v>0.08500000000000001</v>
+        <v>0.08399999999999999</v>
       </c>
       <c r="E2">
-        <v>0.056</v>
+        <v>0.054</v>
       </c>
       <c r="F2">
         <v>0.149</v>
       </c>
       <c r="G2">
-        <v>0.029</v>
+        <v>0.02999999999999999</v>
       </c>
       <c r="H2">
         <v>0.444</v>
@@ -714,13 +714,13 @@
         <v>1.946308724832215</v>
       </c>
       <c r="R2">
-        <v>5.447058823529411</v>
+        <v>5.511904761904762</v>
       </c>
       <c r="S2">
-        <v>0.6964285714285714</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="T2">
-        <v>14.62068965517241</v>
+        <v>14.13333333333334</v>
       </c>
       <c r="U2">
         <v>325729</v>
@@ -764,13 +764,13 @@
         <v>0.054</v>
       </c>
       <c r="E3">
-        <v>0.04500000000000001</v>
+        <v>0.046</v>
       </c>
       <c r="F3">
         <v>0.115</v>
       </c>
       <c r="G3">
-        <v>0.008999999999999994</v>
+        <v>0.008</v>
       </c>
       <c r="H3">
         <v>0.5419999999999999</v>
@@ -806,10 +806,10 @@
         <v>1.37037037037037</v>
       </c>
       <c r="S3">
-        <v>0.8222222222222221</v>
+        <v>0.8043478260869565</v>
       </c>
       <c r="T3">
-        <v>4.111111111111113</v>
+        <v>4.625</v>
       </c>
       <c r="U3">
         <v>317080</v>
@@ -853,13 +853,13 @@
         <v>0.046</v>
       </c>
       <c r="E4">
-        <v>0.046</v>
+        <v>0.048</v>
       </c>
       <c r="F4">
         <v>0.255</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-0.002000000000000002</v>
       </c>
       <c r="H4">
         <v>0.903</v>
@@ -895,7 +895,10 @@
         <v>0.7391304347826088</v>
       </c>
       <c r="S4">
-        <v>0.7391304347826088</v>
+        <v>0.7083333333333334</v>
+      </c>
+      <c r="T4">
+        <v>-0</v>
       </c>
       <c r="U4">
         <v>403394</v>
@@ -933,7 +936,7 @@
         <v>0.115</v>
       </c>
       <c r="D5">
-        <v>0.044</v>
+        <v>0.04500000000000001</v>
       </c>
       <c r="E5">
         <v>0.04500000000000001</v>
@@ -942,7 +945,7 @@
         <v>0.243</v>
       </c>
       <c r="G5">
-        <v>-0.001000000000000008</v>
+        <v>0</v>
       </c>
       <c r="H5">
         <v>0.945</v>
@@ -975,13 +978,13 @@
         <v>1.218106995884774</v>
       </c>
       <c r="R5">
-        <v>0.7272727272727273</v>
+        <v>0.711111111111111</v>
       </c>
       <c r="S5">
         <v>0.7333333333333333</v>
       </c>
-      <c r="T5">
-        <v>0.9999999999999931</v>
+      <c r="T5" t="s">
+        <v>64</v>
       </c>
       <c r="U5">
         <v>1965206</v>
@@ -1019,16 +1022,16 @@
         <v>0.161</v>
       </c>
       <c r="D6">
-        <v>0.203</v>
+        <v>0.221</v>
       </c>
       <c r="E6">
-        <v>0.094</v>
+        <v>0.098</v>
       </c>
       <c r="F6">
         <v>0.871</v>
       </c>
       <c r="G6">
-        <v>0.109</v>
+        <v>0.123</v>
       </c>
       <c r="H6">
         <v>3.856</v>
@@ -1061,13 +1064,13 @@
         <v>3.874856486796785</v>
       </c>
       <c r="R6">
-        <v>3.679802955665024</v>
+        <v>3.380090497737557</v>
       </c>
       <c r="S6">
-        <v>0.4148936170212766</v>
+        <v>0.3979591836734694</v>
       </c>
       <c r="T6">
-        <v>6.495412844036696</v>
+        <v>5.75609756097561</v>
       </c>
       <c r="U6">
         <v>2394385</v>
@@ -1108,16 +1111,16 @@
         <v>0.221</v>
       </c>
       <c r="D7">
-        <v>0.075</v>
+        <v>0.076</v>
       </c>
       <c r="E7">
-        <v>0.067</v>
+        <v>0.06899999999999999</v>
       </c>
       <c r="F7">
         <v>0.878</v>
       </c>
       <c r="G7">
-        <v>0.007999999999999993</v>
+        <v>0.007000000000000006</v>
       </c>
       <c r="H7">
         <v>2.103</v>
@@ -1150,13 +1153,13 @@
         <v>1.657175398633257</v>
       </c>
       <c r="R7">
-        <v>0.8800000000000001</v>
+        <v>0.868421052631579</v>
       </c>
       <c r="S7">
-        <v>0.4776119402985075</v>
+        <v>0.463768115942029</v>
       </c>
       <c r="T7">
-        <v>4.250000000000004</v>
+        <v>4.857142857142853</v>
       </c>
       <c r="U7">
         <v>1224346</v>
@@ -1200,13 +1203,13 @@
         <v>0.177</v>
       </c>
       <c r="E8">
-        <v>0.111</v>
+        <v>0.109</v>
       </c>
       <c r="F8">
         <v>0.8589999999999999</v>
       </c>
       <c r="G8">
-        <v>0.06599999999999999</v>
+        <v>0.06799999999999998</v>
       </c>
       <c r="H8">
         <v>1.828</v>
@@ -1242,10 +1245,10 @@
         <v>4.09039548022599</v>
       </c>
       <c r="S8">
-        <v>0.3783783783783783</v>
+        <v>0.3853211009174311</v>
       </c>
       <c r="T8">
-        <v>10.33333333333334</v>
+        <v>10.02941176470589</v>
       </c>
       <c r="U8">
         <v>685230</v>
@@ -1286,16 +1289,16 @@
         <v>0.385</v>
       </c>
       <c r="D9">
-        <v>0.156</v>
+        <v>0.16</v>
       </c>
       <c r="E9">
-        <v>0.112</v>
+        <v>0.11</v>
       </c>
       <c r="F9">
         <v>1.78</v>
       </c>
       <c r="G9">
-        <v>0.044</v>
+        <v>0.05</v>
       </c>
       <c r="H9">
         <v>4.464</v>
@@ -1328,13 +1331,13 @@
         <v>1.90561797752809</v>
       </c>
       <c r="R9">
-        <v>3.666666666666667</v>
+        <v>3.575</v>
       </c>
       <c r="S9">
-        <v>0.3214285714285715</v>
+        <v>0.3272727272727273</v>
       </c>
       <c r="T9">
-        <v>12.18181818181818</v>
+        <v>10.72</v>
       </c>
       <c r="U9">
         <v>1696415</v>
@@ -1375,16 +1378,16 @@
         <v>0.484</v>
       </c>
       <c r="D10">
-        <v>0.103</v>
+        <v>0.105</v>
       </c>
       <c r="E10">
-        <v>0.102</v>
+        <v>0.104</v>
       </c>
       <c r="F10">
         <v>4.126</v>
       </c>
       <c r="G10">
-        <v>0.001000000000000001</v>
+        <v>0.001000000000000015</v>
       </c>
       <c r="H10">
         <v>7.976999999999999</v>
@@ -1417,10 +1420,10 @@
         <v>1.404507998061076</v>
       </c>
       <c r="R10">
-        <v>0.3106796116504855</v>
+        <v>0.3047619047619047</v>
       </c>
       <c r="S10">
-        <v>0.3137254901960785</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="T10">
         <v>0</v>
@@ -1461,16 +1464,16 @@
         <v>0.642</v>
       </c>
       <c r="D11">
+        <v>0.104</v>
+      </c>
+      <c r="E11">
         <v>0.103</v>
-      </c>
-      <c r="E11">
-        <v>0.104</v>
       </c>
       <c r="F11">
         <v>6.521</v>
       </c>
       <c r="G11">
-        <v>-0.001000000000000001</v>
+        <v>0.001000000000000001</v>
       </c>
       <c r="H11">
         <v>12.62</v>
@@ -1503,13 +1506,13 @@
         <v>1.763993252568624</v>
       </c>
       <c r="R11">
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="S11">
         <v>0.3106796116504855</v>
       </c>
-      <c r="S11">
-        <v>0.3076923076923077</v>
-      </c>
       <c r="T11">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="U11">
         <v>1632803</v>
@@ -1547,7 +1550,7 @@
         <v>0.628</v>
       </c>
       <c r="D12">
-        <v>5.15</v>
+        <v>5.571000000000001</v>
       </c>
       <c r="E12">
         <v>0.43</v>
@@ -1556,7 +1559,7 @@
         <v>15.519</v>
       </c>
       <c r="G12">
-        <v>4.720000000000001</v>
+        <v>5.141000000000001</v>
       </c>
       <c r="H12">
         <v>33.665</v>
@@ -1589,13 +1592,13 @@
         <v>2.076229138475417</v>
       </c>
       <c r="R12">
-        <v>1.306407766990291</v>
+        <v>1.207682642254532</v>
       </c>
       <c r="S12">
         <v>0.7953488372093024</v>
       </c>
       <c r="T12">
-        <v>1.352966101694915</v>
+        <v>1.242170783894184</v>
       </c>
       <c r="U12">
         <v>2601977</v>
@@ -1636,7 +1639,7 @@
         <v>0.889</v>
       </c>
       <c r="D13">
-        <v>0.777</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="E13">
         <v>0.178</v>
@@ -1645,7 +1648,7 @@
         <v>8.172000000000001</v>
       </c>
       <c r="G13">
-        <v>0.599</v>
+        <v>0.631</v>
       </c>
       <c r="H13">
         <v>17.683</v>
@@ -1678,13 +1681,13 @@
         <v>1.878120411160058</v>
       </c>
       <c r="R13">
-        <v>1.808236808236808</v>
+        <v>1.736711990111248</v>
       </c>
       <c r="S13">
         <v>0.4775280898876405</v>
       </c>
       <c r="T13">
-        <v>2.203672787979967</v>
+        <v>2.091917591125198</v>
       </c>
       <c r="U13">
         <v>3997962</v>
@@ -1725,16 +1728,16 @@
         <v>1.037</v>
       </c>
       <c r="D14">
-        <v>1.619</v>
+        <v>1.705</v>
       </c>
       <c r="E14">
-        <v>0.265</v>
+        <v>0.269</v>
       </c>
       <c r="F14">
         <v>11.338</v>
       </c>
       <c r="G14">
-        <v>1.354</v>
+        <v>1.436</v>
       </c>
       <c r="H14">
         <v>23.156</v>
@@ -1767,13 +1770,13 @@
         <v>1.801199506085729</v>
       </c>
       <c r="R14">
-        <v>1.565781346510192</v>
+        <v>1.486803519061584</v>
       </c>
       <c r="S14">
-        <v>0.6981132075471698</v>
+        <v>0.687732342007435</v>
       </c>
       <c r="T14">
-        <v>1.735598227474151</v>
+        <v>1.636490250696379</v>
       </c>
       <c r="U14">
         <v>4847571</v>
@@ -1814,10 +1817,10 @@
         <v>0.983</v>
       </c>
       <c r="D15">
-        <v>0.103</v>
+        <v>0.105</v>
       </c>
       <c r="E15">
-        <v>0.103</v>
+        <v>0.105</v>
       </c>
       <c r="F15">
         <v>3.581</v>
@@ -1856,10 +1859,10 @@
         <v>2.387601228707066</v>
       </c>
       <c r="R15">
-        <v>0.3106796116504855</v>
+        <v>0.3047619047619047</v>
       </c>
       <c r="S15">
-        <v>0.3203883495145631</v>
+        <v>0.3142857142857143</v>
       </c>
       <c r="T15" t="s">
         <v>64</v>
@@ -1900,16 +1903,16 @@
         <v>1.367</v>
       </c>
       <c r="D16">
-        <v>118.771</v>
+        <v>132.114</v>
       </c>
       <c r="E16">
-        <v>2.639</v>
+        <v>2.632</v>
       </c>
       <c r="F16">
         <v>51.355</v>
       </c>
       <c r="G16">
-        <v>116.132</v>
+        <v>129.482</v>
       </c>
       <c r="H16">
         <v>103.449</v>
@@ -1942,13 +1945,13 @@
         <v>1.989134456236004</v>
       </c>
       <c r="R16">
-        <v>1.433481237002298</v>
+        <v>1.288705209137563</v>
       </c>
       <c r="S16">
-        <v>0.9079196665403563</v>
+        <v>0.9103343465045594</v>
       </c>
       <c r="T16">
-        <v>1.44542417249337</v>
+        <v>1.296396410311858</v>
       </c>
       <c r="U16">
         <v>1985306</v>
@@ -1989,16 +1992,16 @@
         <v>2.333</v>
       </c>
       <c r="D17">
-        <v>21.967</v>
+        <v>23.442</v>
       </c>
       <c r="E17">
-        <v>1.181</v>
+        <v>1.179</v>
       </c>
       <c r="F17">
         <v>51.966</v>
       </c>
       <c r="G17">
-        <v>20.786</v>
+        <v>22.263</v>
       </c>
       <c r="H17">
         <v>95.11799999999999</v>
@@ -2031,13 +2034,13 @@
         <v>1.786629719431936</v>
       </c>
       <c r="R17">
-        <v>1.1959757818546</v>
+        <v>1.120723487757017</v>
       </c>
       <c r="S17">
-        <v>0.8789161727349704</v>
+        <v>0.8804071246819341</v>
       </c>
       <c r="T17">
-        <v>1.213990185701915</v>
+        <v>1.133450119031577</v>
       </c>
       <c r="U17">
         <v>3072441</v>
@@ -2078,16 +2081,16 @@
         <v>3.458</v>
       </c>
       <c r="D18">
-        <v>10.155</v>
+        <v>10.957</v>
       </c>
       <c r="E18">
-        <v>1.125</v>
+        <v>1.124</v>
       </c>
       <c r="F18">
         <v>64.69600000000001</v>
       </c>
       <c r="G18">
-        <v>9.030000000000001</v>
+        <v>9.832999999999998</v>
       </c>
       <c r="H18">
         <v>120.842</v>
@@ -2120,13 +2123,13 @@
         <v>1.789631507357487</v>
       </c>
       <c r="R18">
-        <v>1.260068931560807</v>
+        <v>1.167837911837182</v>
       </c>
       <c r="S18">
-        <v>0.9031111111111111</v>
+        <v>0.9039145907473309</v>
       </c>
       <c r="T18">
-        <v>1.30454042081949</v>
+        <v>1.198006712091936</v>
       </c>
       <c r="U18">
         <v>6783976</v>
@@ -2167,16 +2170,16 @@
         <v>3.573</v>
       </c>
       <c r="D19">
-        <v>0.103</v>
+        <v>0.105</v>
       </c>
       <c r="E19">
-        <v>0.103</v>
+        <v>0.104</v>
       </c>
       <c r="F19">
         <v>13.851</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>0.001000000000000015</v>
       </c>
       <c r="H19">
         <v>90.05199999999999</v>
@@ -2209,10 +2212,13 @@
         <v>2.39513392534835</v>
       </c>
       <c r="R19">
-        <v>0.3106796116504855</v>
+        <v>0.3047619047619047</v>
       </c>
       <c r="S19">
-        <v>0.3106796116504855</v>
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
       </c>
       <c r="U19">
         <v>214005017</v>
@@ -2250,16 +2256,16 @@
         <v>15.506</v>
       </c>
       <c r="D20">
-        <v>2152.196</v>
+        <v>2234.056</v>
       </c>
       <c r="E20">
-        <v>18.526</v>
+        <v>18.519</v>
       </c>
       <c r="F20">
         <v>642.926</v>
       </c>
       <c r="G20">
-        <v>2133.67</v>
+        <v>2215.537</v>
       </c>
       <c r="H20">
         <v>1052.011</v>
@@ -2292,13 +2298,13 @@
         <v>1.592074360035214</v>
       </c>
       <c r="R20">
-        <v>1.18658663058569</v>
+        <v>1.143107871960237</v>
       </c>
       <c r="S20">
-        <v>0.8718557702688114</v>
+        <v>0.8721853231815972</v>
       </c>
       <c r="T20">
-        <v>1.189319341791374</v>
+        <v>1.14537243115326</v>
       </c>
       <c r="U20">
         <v>41652230</v>
@@ -2339,16 +2345,16 @@
         <v>25.867</v>
       </c>
       <c r="D21">
-        <v>872.9400000000001</v>
+        <v>902.676</v>
       </c>
       <c r="E21">
-        <v>37.256</v>
+        <v>37.258</v>
       </c>
       <c r="F21">
         <v>1006.562</v>
       </c>
       <c r="G21">
-        <v>835.6840000000001</v>
+        <v>865.418</v>
       </c>
       <c r="H21">
         <v>1756.588</v>
@@ -2381,13 +2387,13 @@
         <v>1.709270765238505</v>
       </c>
       <c r="R21">
-        <v>1.073773684331111</v>
+        <v>1.038401375465837</v>
       </c>
       <c r="S21">
-        <v>0.9472299763796436</v>
+        <v>0.9471791293145095</v>
       </c>
       <c r="T21">
-        <v>1.079415185644334</v>
+        <v>1.042328678164771</v>
       </c>
       <c r="U21">
         <v>65608366</v>
@@ -2428,7 +2434,7 @@
         <v>0.123</v>
       </c>
       <c r="D22">
-        <v>0.073</v>
+        <v>0.076</v>
       </c>
       <c r="E22">
         <v>0.051</v>
@@ -2437,7 +2443,7 @@
         <v>0.787</v>
       </c>
       <c r="G22">
-        <v>0.022</v>
+        <v>0.025</v>
       </c>
       <c r="H22">
         <v>2.54</v>
@@ -2470,13 +2476,13 @@
         <v>2.950444726810673</v>
       </c>
       <c r="R22">
-        <v>4.26027397260274</v>
+        <v>4.092105263157895</v>
       </c>
       <c r="S22">
         <v>0.6862745098039216</v>
       </c>
       <c r="T22">
-        <v>12.54545454545455</v>
+        <v>11.04</v>
       </c>
       <c r="U22">
         <v>358937</v>
@@ -2517,16 +2523,16 @@
         <v>0.203</v>
       </c>
       <c r="D23">
-        <v>0.515</v>
+        <v>0.5720000000000001</v>
       </c>
       <c r="E23">
-        <v>0.142</v>
+        <v>0.145</v>
       </c>
       <c r="F23">
         <v>1.838</v>
       </c>
       <c r="G23">
-        <v>0.373</v>
+        <v>0.427</v>
       </c>
       <c r="H23">
         <v>5.774</v>
@@ -2559,13 +2565,13 @@
         <v>2.983133841131665</v>
       </c>
       <c r="R23">
-        <v>2.293203883495146</v>
+        <v>2.064685314685315</v>
       </c>
       <c r="S23">
-        <v>0.4718309859154929</v>
+        <v>0.4620689655172414</v>
       </c>
       <c r="T23">
-        <v>2.986595174262735</v>
+        <v>2.608899297423887</v>
       </c>
       <c r="U23">
         <v>456857</v>
@@ -2606,16 +2612,16 @@
         <v>0.227</v>
       </c>
       <c r="D24">
-        <v>3.238</v>
+        <v>3.651</v>
       </c>
       <c r="E24">
-        <v>0.287</v>
+        <v>0.291</v>
       </c>
       <c r="F24">
         <v>4.501</v>
       </c>
       <c r="G24">
-        <v>2.951</v>
+        <v>3.36</v>
       </c>
       <c r="H24">
         <v>11.562</v>
@@ -2648,13 +2654,13 @@
         <v>2.494778938013774</v>
       </c>
       <c r="R24">
-        <v>1.516059295861643</v>
+        <v>1.344563133388113</v>
       </c>
       <c r="S24">
-        <v>0.7212543554006969</v>
+        <v>0.7113402061855669</v>
       </c>
       <c r="T24">
-        <v>1.593358183666554</v>
+        <v>1.399404761904762</v>
       </c>
       <c r="U24">
         <v>559175</v>
@@ -2695,7 +2701,7 @@
         <v>0.296</v>
       </c>
       <c r="D25">
-        <v>14.365</v>
+        <v>15.806</v>
       </c>
       <c r="E25">
         <v>0.467</v>
@@ -2704,7 +2710,7 @@
         <v>12.678</v>
       </c>
       <c r="G25">
-        <v>13.898</v>
+        <v>15.339</v>
       </c>
       <c r="H25">
         <v>31.954</v>
@@ -2737,13 +2743,13 @@
         <v>2.490061523899669</v>
       </c>
       <c r="R25">
-        <v>1.329342151061608</v>
+        <v>1.20814880425155</v>
       </c>
       <c r="S25">
         <v>0.7922912205567452</v>
       </c>
       <c r="T25">
-        <v>1.347388113397611</v>
+        <v>1.220809700762761</v>
       </c>
       <c r="U25">
         <v>660444</v>
@@ -2784,16 +2790,16 @@
         <v>0.388</v>
       </c>
       <c r="D26">
-        <v>57.76499999999999</v>
+        <v>62.473</v>
       </c>
       <c r="E26">
-        <v>0.695</v>
+        <v>0.6920000000000001</v>
       </c>
       <c r="F26">
         <v>32.361</v>
       </c>
       <c r="G26">
-        <v>57.06999999999999</v>
+        <v>61.781</v>
       </c>
       <c r="H26">
         <v>70.97399999999999</v>
@@ -2826,13 +2832,13 @@
         <v>2.179073576218287</v>
       </c>
       <c r="R26">
-        <v>1.28660953864797</v>
+        <v>1.189649928769228</v>
       </c>
       <c r="S26">
-        <v>0.7884892086330935</v>
+        <v>0.7919075144508669</v>
       </c>
       <c r="T26">
-        <v>1.292675661468372</v>
+        <v>1.194104983732863</v>
       </c>
       <c r="U26">
         <v>755026</v>
@@ -2873,16 +2879,16 @@
         <v>0.388</v>
       </c>
       <c r="D27">
-        <v>57.76499999999999</v>
+        <v>62.473</v>
       </c>
       <c r="E27">
-        <v>0.695</v>
+        <v>0.6920000000000001</v>
       </c>
       <c r="F27">
         <v>32.361</v>
       </c>
       <c r="G27">
-        <v>57.06999999999999</v>
+        <v>61.781</v>
       </c>
       <c r="H27">
         <v>70.97399999999999</v>
@@ -2915,13 +2921,13 @@
         <v>2.179073576218287</v>
       </c>
       <c r="R27">
-        <v>1.28660953864797</v>
+        <v>1.189649928769228</v>
       </c>
       <c r="S27">
-        <v>0.7884892086330935</v>
+        <v>0.7919075144508669</v>
       </c>
       <c r="T27">
-        <v>1.292675661468372</v>
+        <v>1.194104983732863</v>
       </c>
       <c r="U27">
         <v>755026</v>
@@ -2962,16 +2968,16 @@
         <v>0.388</v>
       </c>
       <c r="D28">
-        <v>57.76499999999999</v>
+        <v>62.473</v>
       </c>
       <c r="E28">
-        <v>0.695</v>
+        <v>0.6920000000000001</v>
       </c>
       <c r="F28">
         <v>32.361</v>
       </c>
       <c r="G28">
-        <v>57.06999999999999</v>
+        <v>61.781</v>
       </c>
       <c r="H28">
         <v>70.968</v>
@@ -3004,13 +3010,13 @@
         <v>2.17888816785637</v>
       </c>
       <c r="R28">
-        <v>1.286817276897776</v>
+        <v>1.189842011749076</v>
       </c>
       <c r="S28">
-        <v>0.7884892086330935</v>
+        <v>0.7919075144508669</v>
       </c>
       <c r="T28">
-        <v>1.292885929560189</v>
+        <v>1.194299218206245</v>
       </c>
       <c r="U28">
         <v>755026</v>
@@ -3051,16 +3057,16 @@
         <v>0.388</v>
       </c>
       <c r="D29">
-        <v>57.76499999999999</v>
+        <v>62.473</v>
       </c>
       <c r="E29">
-        <v>0.695</v>
+        <v>0.6920000000000001</v>
       </c>
       <c r="F29">
         <v>32.361</v>
       </c>
       <c r="G29">
-        <v>57.06999999999999</v>
+        <v>61.781</v>
       </c>
       <c r="H29">
         <v>70.968</v>
@@ -3093,13 +3099,13 @@
         <v>2.17888816785637</v>
       </c>
       <c r="R29">
-        <v>1.286817276897776</v>
+        <v>1.189842011749076</v>
       </c>
       <c r="S29">
-        <v>0.7884892086330935</v>
+        <v>0.7919075144508669</v>
       </c>
       <c r="T29">
-        <v>1.292885929560189</v>
+        <v>1.194299218206245</v>
       </c>
       <c r="U29">
         <v>755026</v>
@@ -3140,16 +3146,16 @@
         <v>0.378</v>
       </c>
       <c r="D30">
-        <v>236.095</v>
+        <v>249.379</v>
       </c>
       <c r="E30">
-        <v>1.491</v>
+        <v>1.492</v>
       </c>
       <c r="F30">
         <v>51.46</v>
       </c>
       <c r="G30">
-        <v>234.604</v>
+        <v>247.887</v>
       </c>
       <c r="H30">
         <v>100.09</v>
@@ -3182,13 +3188,13 @@
         <v>1.935814224640497</v>
       </c>
       <c r="R30">
-        <v>1.246261038988543</v>
+        <v>1.17987480902562</v>
       </c>
       <c r="S30">
-        <v>0.8202548625083836</v>
+        <v>0.8197050938337801</v>
       </c>
       <c r="T30">
-        <v>1.248968474535814</v>
+        <v>1.182042624260248</v>
       </c>
       <c r="U30">
         <v>837036</v>
@@ -3229,16 +3235,16 @@
         <v>0.41</v>
       </c>
       <c r="D31">
-        <v>785.628</v>
+        <v>815.6940000000001</v>
       </c>
       <c r="E31">
-        <v>2.618</v>
+        <v>2.616</v>
       </c>
       <c r="F31">
         <v>91.34800000000001</v>
       </c>
       <c r="G31">
-        <v>783.01</v>
+        <v>813.0780000000001</v>
       </c>
       <c r="H31">
         <v>186.373</v>
@@ -3271,13 +3277,13 @@
         <v>2.034987082366335</v>
       </c>
       <c r="R31">
-        <v>1.247920135229396</v>
+        <v>1.201922534675994</v>
       </c>
       <c r="S31">
-        <v>0.7983193277310924</v>
+        <v>0.7989296636085628</v>
       </c>
       <c r="T31">
-        <v>1.249423379011762</v>
+        <v>1.203219125348367</v>
       </c>
       <c r="U31">
         <v>904525</v>
@@ -3318,16 +3324,16 @@
         <v>0.53</v>
       </c>
       <c r="D32">
-        <v>2420.24</v>
+        <v>2477.632</v>
       </c>
       <c r="E32">
-        <v>3.85</v>
+        <v>3.851</v>
       </c>
       <c r="F32">
         <v>207.092</v>
       </c>
       <c r="G32">
-        <v>2416.39</v>
+        <v>2473.780999999999</v>
       </c>
       <c r="H32">
         <v>393.392</v>
@@ -3360,13 +3366,13 @@
         <v>1.897084387615166</v>
       </c>
       <c r="R32">
-        <v>1.264769196443328</v>
+        <v>1.235472015214528</v>
       </c>
       <c r="S32">
-        <v>0.737922077922078</v>
+        <v>0.7377304596208778</v>
       </c>
       <c r="T32">
-        <v>1.265608614503453</v>
+        <v>1.236246862596164</v>
       </c>
       <c r="U32">
         <v>955990</v>
@@ -3407,7 +3413,7 @@
         <v>0.148</v>
       </c>
       <c r="D33">
-        <v>2.004</v>
+        <v>2.342</v>
       </c>
       <c r="E33">
         <v>0.187</v>
@@ -3416,7 +3422,7 @@
         <v>1.743</v>
       </c>
       <c r="G33">
-        <v>1.817</v>
+        <v>2.155</v>
       </c>
       <c r="H33">
         <v>7.715</v>
@@ -3449,13 +3455,13 @@
         <v>4.378083763625932</v>
       </c>
       <c r="R33">
-        <v>1.852295409181637</v>
+        <v>1.584970111016226</v>
       </c>
       <c r="S33">
         <v>0.5935828877005348</v>
       </c>
       <c r="T33">
-        <v>1.981838194826637</v>
+        <v>1.670997679814385</v>
       </c>
       <c r="U33">
         <v>102869</v>
@@ -3496,7 +3502,7 @@
         <v>0.195</v>
       </c>
       <c r="D34">
-        <v>6.021</v>
+        <v>6.834</v>
       </c>
       <c r="E34">
         <v>0.256</v>
@@ -3505,7 +3511,7 @@
         <v>5.145</v>
       </c>
       <c r="G34">
-        <v>5.765</v>
+        <v>6.577999999999999</v>
       </c>
       <c r="H34">
         <v>18.753</v>
@@ -3538,13 +3544,13 @@
         <v>3.616909620991254</v>
       </c>
       <c r="R34">
-        <v>1.527154957648231</v>
+        <v>1.345478489903424</v>
       </c>
       <c r="S34">
         <v>0.67578125</v>
       </c>
       <c r="T34">
-        <v>1.564960971379011</v>
+        <v>1.371541501976285</v>
       </c>
       <c r="U34">
         <v>199881</v>
@@ -3585,7 +3591,7 @@
         <v>0.226</v>
       </c>
       <c r="D35">
-        <v>22.528</v>
+        <v>24.72</v>
       </c>
       <c r="E35">
         <v>0.508</v>
@@ -3594,7 +3600,7 @@
         <v>9.887999999999998</v>
       </c>
       <c r="G35">
-        <v>22.02</v>
+        <v>24.212</v>
       </c>
       <c r="H35">
         <v>23.511</v>
@@ -3627,13 +3633,13 @@
         <v>2.353762135922331</v>
       </c>
       <c r="R35">
-        <v>1.328746448863636</v>
+        <v>1.210922330097087</v>
       </c>
       <c r="S35">
         <v>0.7874015748031497</v>
       </c>
       <c r="T35">
-        <v>1.341235240690281</v>
+        <v>1.219808359491161</v>
       </c>
       <c r="U35">
         <v>388707</v>
@@ -3674,7 +3680,7 @@
         <v>0.389</v>
       </c>
       <c r="D36">
-        <v>57.812</v>
+        <v>62.466</v>
       </c>
       <c r="E36">
         <v>0.6920000000000001</v>
@@ -3683,7 +3689,7 @@
         <v>32.363</v>
       </c>
       <c r="G36">
-        <v>57.12</v>
+        <v>61.774</v>
       </c>
       <c r="H36">
         <v>70.97399999999999</v>
@@ -3716,13 +3722,13 @@
         <v>2.178938911720174</v>
       </c>
       <c r="R36">
-        <v>1.285563550819899</v>
+        <v>1.189783242083694</v>
       </c>
       <c r="S36">
         <v>0.7919075144508669</v>
       </c>
       <c r="T36">
-        <v>1.291544117647059</v>
+        <v>1.194240295269855</v>
       </c>
       <c r="U36">
         <v>755026</v>
@@ -3763,7 +3769,7 @@
         <v>0.389</v>
       </c>
       <c r="D37">
-        <v>57.812</v>
+        <v>62.466</v>
       </c>
       <c r="E37">
         <v>0.6920000000000001</v>
@@ -3772,7 +3778,7 @@
         <v>32.363</v>
       </c>
       <c r="G37">
-        <v>57.12</v>
+        <v>61.774</v>
       </c>
       <c r="H37">
         <v>70.97399999999999</v>
@@ -3805,13 +3811,13 @@
         <v>2.178938911720174</v>
       </c>
       <c r="R37">
-        <v>1.285563550819899</v>
+        <v>1.189783242083694</v>
       </c>
       <c r="S37">
         <v>0.7919075144508669</v>
       </c>
       <c r="T37">
-        <v>1.291544117647059</v>
+        <v>1.194240295269855</v>
       </c>
       <c r="U37">
         <v>755026</v>
@@ -3852,7 +3858,7 @@
         <v>0.389</v>
       </c>
       <c r="D38">
-        <v>57.812</v>
+        <v>62.466</v>
       </c>
       <c r="E38">
         <v>0.6920000000000001</v>
@@ -3861,7 +3867,7 @@
         <v>32.363</v>
       </c>
       <c r="G38">
-        <v>57.12</v>
+        <v>61.774</v>
       </c>
       <c r="H38">
         <v>70.968</v>
@@ -3894,13 +3900,13 @@
         <v>2.178753514816303</v>
       </c>
       <c r="R38">
-        <v>1.285771120182661</v>
+        <v>1.189975346588544</v>
       </c>
       <c r="S38">
         <v>0.7919075144508669</v>
       </c>
       <c r="T38">
-        <v>1.291754201680672</v>
+        <v>1.194434551753165</v>
       </c>
       <c r="U38">
         <v>755026</v>
@@ -3941,7 +3947,7 @@
         <v>0.389</v>
       </c>
       <c r="D39">
-        <v>57.812</v>
+        <v>62.466</v>
       </c>
       <c r="E39">
         <v>0.6920000000000001</v>
@@ -3950,7 +3956,7 @@
         <v>32.363</v>
       </c>
       <c r="G39">
-        <v>57.12</v>
+        <v>61.774</v>
       </c>
       <c r="H39">
         <v>70.968</v>
@@ -3983,13 +3989,13 @@
         <v>2.178753514816303</v>
       </c>
       <c r="R39">
-        <v>1.285771120182661</v>
+        <v>1.189975346588544</v>
       </c>
       <c r="S39">
         <v>0.7919075144508669</v>
       </c>
       <c r="T39">
-        <v>1.291754201680672</v>
+        <v>1.194434551753165</v>
       </c>
       <c r="U39">
         <v>755026</v>
@@ -4030,16 +4036,16 @@
         <v>0.465</v>
       </c>
       <c r="D40">
-        <v>193.099</v>
+        <v>204.991</v>
       </c>
       <c r="E40">
-        <v>1.896</v>
+        <v>1.897</v>
       </c>
       <c r="F40">
         <v>54.06699999999999</v>
       </c>
       <c r="G40">
-        <v>191.203</v>
+        <v>203.094</v>
       </c>
       <c r="H40">
         <v>101.223</v>
@@ -4072,13 +4078,13 @@
         <v>1.857676586457544</v>
       </c>
       <c r="R40">
-        <v>1.213232590536461</v>
+        <v>1.142850173910074</v>
       </c>
       <c r="S40">
-        <v>0.8628691983122364</v>
+        <v>0.8624143384290986</v>
       </c>
       <c r="T40">
-        <v>1.21670685083393</v>
+        <v>1.145469585512127</v>
       </c>
       <c r="U40">
         <v>1465546</v>
@@ -4119,7 +4125,7 @@
         <v>0.907</v>
       </c>
       <c r="D41">
-        <v>489.734</v>
+        <v>515.397</v>
       </c>
       <c r="E41">
         <v>2.897</v>
@@ -4128,7 +4134,7 @@
         <v>163.63</v>
       </c>
       <c r="G41">
-        <v>486.837</v>
+        <v>512.5</v>
       </c>
       <c r="H41">
         <v>290.896</v>
@@ -4161,13 +4167,13 @@
         <v>1.768263765813115</v>
       </c>
       <c r="R41">
-        <v>1.20333691350815</v>
+        <v>1.143419538724517</v>
       </c>
       <c r="S41">
         <v>0.8429409734207802</v>
       </c>
       <c r="T41">
-        <v>1.205481506130389</v>
+        <v>1.145118048780488</v>
       </c>
       <c r="U41">
         <v>2845797</v>
@@ -4208,16 +4214,16 @@
         <v>1.959</v>
       </c>
       <c r="D42">
-        <v>1210.892</v>
+        <v>1264.359</v>
       </c>
       <c r="E42">
-        <v>4.505999999999999</v>
+        <v>4.507</v>
       </c>
       <c r="F42">
         <v>499.409</v>
       </c>
       <c r="G42">
-        <v>1206.386</v>
+        <v>1259.852</v>
       </c>
       <c r="H42">
         <v>899</v>
@@ -4250,13 +4256,13 @@
         <v>1.793918411562467</v>
       </c>
       <c r="R42">
-        <v>1.207073793534023</v>
+        <v>1.156029260676754</v>
       </c>
       <c r="S42">
-        <v>0.8071460275188639</v>
+        <v>0.8069669403150656</v>
       </c>
       <c r="T42">
-        <v>1.208567572899553</v>
+        <v>1.157277997733067</v>
       </c>
       <c r="U42">
         <v>5520326</v>
@@ -4297,16 +4303,16 @@
         <v>2.458</v>
       </c>
       <c r="D43">
-        <v>3643.182</v>
+        <v>3797.544</v>
       </c>
       <c r="E43">
-        <v>12.876</v>
+        <v>12.875</v>
       </c>
       <c r="F43">
         <v>785.4250000000001</v>
       </c>
       <c r="G43">
-        <v>3630.306</v>
+        <v>3784.669</v>
       </c>
       <c r="H43">
         <v>1270.524</v>
@@ -4339,13 +4345,13 @@
         <v>1.610660470445937</v>
       </c>
       <c r="R43">
-        <v>1.193425966641249</v>
+        <v>1.144915766611263</v>
       </c>
       <c r="S43">
-        <v>0.8561665113389252</v>
+        <v>0.8562330097087379</v>
       </c>
       <c r="T43">
-        <v>1.194622161327447</v>
+        <v>1.145897831488038</v>
       </c>
       <c r="U43">
         <v>10708196</v>

</xml_diff>